<commit_message>
World category update enable func test
</commit_message>
<xml_diff>
--- a/na-service/src/main/resources/data/category/Categories.xlsx
+++ b/na-service/src/main/resources/data/category/Categories.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="366">
   <si>
     <t>name</t>
   </si>
@@ -689,6 +689,12 @@
     <t>Volleyball</t>
   </si>
   <si>
+    <t>covid-19</t>
+  </si>
+  <si>
+    <t>Covid-19</t>
+  </si>
+  <si>
     <t>World</t>
   </si>
   <si>
@@ -1038,13 +1044,79 @@
   </si>
   <si>
     <t>Hua Hin</t>
+  </si>
+  <si>
+    <t>guatemala</t>
+  </si>
+  <si>
+    <t>Гватемала</t>
+  </si>
+  <si>
+    <t>Guatemala</t>
+  </si>
+  <si>
+    <t>argentina</t>
+  </si>
+  <si>
+    <t>latin</t>
+  </si>
+  <si>
+    <t>Аргентина</t>
+  </si>
+  <si>
+    <t>Argentina</t>
+  </si>
+  <si>
+    <t>mexico</t>
+  </si>
+  <si>
+    <t>Мексика</t>
+  </si>
+  <si>
+    <t>Mexico</t>
+  </si>
+  <si>
+    <t>brazil</t>
+  </si>
+  <si>
+    <t>Бразилия</t>
+  </si>
+  <si>
+    <t>Brazil</t>
+  </si>
+  <si>
+    <t>Бразилія</t>
+  </si>
+  <si>
+    <t>honduras</t>
+  </si>
+  <si>
+    <t>Гондурас</t>
+  </si>
+  <si>
+    <t>Honduras</t>
+  </si>
+  <si>
+    <t>egypt</t>
+  </si>
+  <si>
+    <t>africa</t>
+  </si>
+  <si>
+    <t>Египет</t>
+  </si>
+  <si>
+    <t>Egypt</t>
+  </si>
+  <si>
+    <t>Єгипет</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -1058,6 +1130,9 @@
     <font>
       <sz val="13.0"/>
       <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
       <name val="Arial"/>
     </font>
     <font>
@@ -1085,7 +1160,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1107,7 +1182,10 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -2448,13 +2526,13 @@
       <c r="B69" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="C69" s="2" t="s">
+      <c r="C69" s="7" t="s">
         <v>131</v>
       </c>
       <c r="D69" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="E69" s="2" t="s">
+      <c r="E69" s="7" t="s">
         <v>131</v>
       </c>
     </row>
@@ -2561,7 +2639,7 @@
       </c>
     </row>
     <row r="76">
-      <c r="A76" s="7" t="s">
+      <c r="A76" s="8" t="s">
         <v>211</v>
       </c>
       <c r="B76" s="1" t="s">
@@ -2623,6 +2701,20 @@
       </c>
       <c r="E79" s="2" t="s">
         <v>223</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>226</v>
       </c>
     </row>
   </sheetData>
@@ -2659,662 +2751,746 @@
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>228</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>225</v>
+        <v>230</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>225</v>
+        <v>238</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>225</v>
+        <v>241</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>239</v>
-      </c>
       <c r="C8" s="2" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>225</v>
+        <v>248</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>225</v>
+        <v>250</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>225</v>
+        <v>253</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>340</v>
+        <v>342</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>365</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added news note notification entity added Bali category added coconut news dropped notify-queue
</commit_message>
<xml_diff>
--- a/na-service/src/main/resources/data/category/Categories.xlsx
+++ b/na-service/src/main/resources/data/category/Categories.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="366">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="371">
   <si>
     <t>name</t>
   </si>
@@ -623,72 +623,72 @@
     <t>Boxing</t>
   </si>
   <si>
+    <t>hockey</t>
+  </si>
+  <si>
+    <t>Хоккей</t>
+  </si>
+  <si>
+    <t>Hockey</t>
+  </si>
+  <si>
+    <t>Хокей</t>
+  </si>
+  <si>
+    <t>chess</t>
+  </si>
+  <si>
+    <t>Шахматы</t>
+  </si>
+  <si>
+    <t>Chess</t>
+  </si>
+  <si>
+    <t>Шахи</t>
+  </si>
+  <si>
+    <t>food-lifestyle</t>
+  </si>
+  <si>
+    <t>Еда и напитки</t>
+  </si>
+  <si>
+    <t>Food and drinks</t>
+  </si>
+  <si>
+    <t>Їжа та напої</t>
+  </si>
+  <si>
+    <t>positive</t>
+  </si>
+  <si>
+    <t>Позитивные</t>
+  </si>
+  <si>
+    <t>Positive</t>
+  </si>
+  <si>
+    <t>Позитивні</t>
+  </si>
+  <si>
+    <t>volleyball</t>
+  </si>
+  <si>
+    <t>Волейбол</t>
+  </si>
+  <si>
+    <t>Volleyball</t>
+  </si>
+  <si>
     <t>basketball</t>
   </si>
   <si>
-    <t>Хоккей</t>
-  </si>
-  <si>
-    <t>Hockey</t>
-  </si>
-  <si>
-    <t>Хокей</t>
-  </si>
-  <si>
-    <t>hockey</t>
-  </si>
-  <si>
-    <t>Шахматы</t>
-  </si>
-  <si>
-    <t>Chess</t>
-  </si>
-  <si>
-    <t>Шахи</t>
-  </si>
-  <si>
-    <t>chess</t>
-  </si>
-  <si>
-    <t>Еда и напитки</t>
-  </si>
-  <si>
-    <t>Food and drinks</t>
-  </si>
-  <si>
-    <t>Їжа та напої</t>
-  </si>
-  <si>
-    <t>food-lifestyle</t>
-  </si>
-  <si>
-    <t>Позитивные</t>
-  </si>
-  <si>
-    <t>Positive</t>
-  </si>
-  <si>
-    <t>Позитивні</t>
-  </si>
-  <si>
-    <t>positive</t>
-  </si>
-  <si>
     <t>Баскетбол</t>
   </si>
   <si>
     <t>Basketball</t>
   </si>
   <si>
-    <t>volleyball</t>
-  </si>
-  <si>
-    <t>Волейбол</t>
-  </si>
-  <si>
-    <t>Volleyball</t>
-  </si>
-  <si>
     <t>covid-19</t>
   </si>
   <si>
@@ -1110,13 +1110,28 @@
   </si>
   <si>
     <t>Єгипет</t>
+  </si>
+  <si>
+    <t>bali</t>
+  </si>
+  <si>
+    <t>asia</t>
+  </si>
+  <si>
+    <t>Бали</t>
+  </si>
+  <si>
+    <t>Bali</t>
+  </si>
+  <si>
+    <t>Балі</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -1126,19 +1141,16 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
-    <font/>
     <font>
       <sz val="13.0"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
-      <name val="Arial"/>
-    </font>
-    <font>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
+    <font/>
   </fonts>
   <fills count="3">
     <fill>
@@ -1160,7 +1172,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1173,19 +1185,16 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -1429,7 +1438,7 @@
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -1443,7 +1452,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -1460,7 +1469,7 @@
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -1477,7 +1486,7 @@
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -1683,10 +1692,10 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="1" t="s">
         <v>51</v>
       </c>
       <c r="C18" s="2" t="s">
@@ -1892,13 +1901,13 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="4" t="s">
+      <c r="A31" s="3" t="s">
         <v>51</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="D31" s="5" t="s">
+      <c r="D31" s="4" t="s">
         <v>51</v>
       </c>
       <c r="E31" s="2" t="s">
@@ -2056,7 +2065,7 @@
       <c r="A41" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="B41" s="3" t="s">
         <v>51</v>
       </c>
       <c r="C41" s="2" t="s">
@@ -2486,7 +2495,7 @@
       </c>
     </row>
     <row r="67">
-      <c r="A67" s="6" t="s">
+      <c r="A67" s="5" t="s">
         <v>184</v>
       </c>
       <c r="B67" s="1" t="s">
@@ -2503,7 +2512,7 @@
       </c>
     </row>
     <row r="68">
-      <c r="A68" s="6" t="s">
+      <c r="A68" s="5" t="s">
         <v>188</v>
       </c>
       <c r="B68" s="1" t="s">
@@ -2526,13 +2535,13 @@
       <c r="B69" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="C69" s="7" t="s">
+      <c r="C69" s="2" t="s">
         <v>131</v>
       </c>
       <c r="D69" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="E69" s="7" t="s">
+      <c r="E69" s="2" t="s">
         <v>131</v>
       </c>
     </row>
@@ -2609,7 +2618,7 @@
         <v>203</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>108</v>
+        <v>170</v>
       </c>
       <c r="C74" s="2" t="s">
         <v>204</v>
@@ -2622,11 +2631,11 @@
       </c>
     </row>
     <row r="75">
-      <c r="A75" s="1" t="s">
+      <c r="A75" s="6" t="s">
         <v>207</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>170</v>
+        <v>108</v>
       </c>
       <c r="C75" s="2" t="s">
         <v>208</v>
@@ -2639,11 +2648,11 @@
       </c>
     </row>
     <row r="76">
-      <c r="A76" s="8" t="s">
+      <c r="A76" s="1" t="s">
         <v>211</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>108</v>
+        <v>51</v>
       </c>
       <c r="C76" s="2" t="s">
         <v>212</v>
@@ -2659,9 +2668,6 @@
       <c r="A77" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="B77" s="1" t="s">
-        <v>51</v>
-      </c>
       <c r="C77" s="2" t="s">
         <v>216</v>
       </c>
@@ -2676,6 +2682,9 @@
       <c r="A78" s="1" t="s">
         <v>219</v>
       </c>
+      <c r="B78" s="1" t="s">
+        <v>108</v>
+      </c>
       <c r="C78" s="2" t="s">
         <v>220</v>
       </c>
@@ -2704,7 +2713,7 @@
       </c>
     </row>
     <row r="80">
-      <c r="A80" s="3" t="s">
+      <c r="A80" s="1" t="s">
         <v>225</v>
       </c>
       <c r="C80" s="1" t="s">
@@ -2750,7 +2759,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="1" t="s">
         <v>227</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -2764,7 +2773,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="1" t="s">
         <v>230</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -3412,7 +3421,7 @@
       <c r="A42" s="1" t="s">
         <v>347</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="B42" s="1" t="s">
         <v>348</v>
       </c>
       <c r="C42" s="1" t="s">
@@ -3460,7 +3469,7 @@
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="3" t="s">
+      <c r="A45" s="1" t="s">
         <v>358</v>
       </c>
       <c r="B45" s="1" t="s">
@@ -3491,6 +3500,23 @@
       </c>
       <c r="E46" s="1" t="s">
         <v>365</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>367</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>370</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Russia without parent now
</commit_message>
<xml_diff>
--- a/na-service/src/main/resources/data/category/Categories.xlsx
+++ b/na-service/src/main/resources/data/category/Categories.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="403">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="407">
   <si>
     <t>name</t>
   </si>
@@ -875,99 +875,99 @@
     <t>Italy</t>
   </si>
   <si>
+    <t>Италия</t>
+  </si>
+  <si>
+    <t>Італія</t>
+  </si>
+  <si>
+    <t>France</t>
+  </si>
+  <si>
+    <t>Франция</t>
+  </si>
+  <si>
+    <t>Франція</t>
+  </si>
+  <si>
+    <t>Greece</t>
+  </si>
+  <si>
+    <t>Греция</t>
+  </si>
+  <si>
+    <t>Греція</t>
+  </si>
+  <si>
+    <t>Germany</t>
+  </si>
+  <si>
+    <t>Германия</t>
+  </si>
+  <si>
+    <t>Германія</t>
+  </si>
+  <si>
+    <t>Denmark</t>
+  </si>
+  <si>
+    <t>Дания</t>
+  </si>
+  <si>
+    <t>Данія</t>
+  </si>
+  <si>
+    <t>Sweden</t>
+  </si>
+  <si>
+    <t>Швеция</t>
+  </si>
+  <si>
+    <t>Швеція</t>
+  </si>
+  <si>
+    <t>Norway</t>
+  </si>
+  <si>
+    <t>Норвегия</t>
+  </si>
+  <si>
+    <t>Норвегія</t>
+  </si>
+  <si>
+    <t>Finland</t>
+  </si>
+  <si>
+    <t>Финляндия</t>
+  </si>
+  <si>
+    <t>Фінляндія</t>
+  </si>
+  <si>
+    <t>Spain</t>
+  </si>
+  <si>
+    <t>Испания</t>
+  </si>
+  <si>
+    <t>Іспанія</t>
+  </si>
+  <si>
+    <t>Austria</t>
+  </si>
+  <si>
+    <t>Австрия</t>
+  </si>
+  <si>
+    <t>Австрія</t>
+  </si>
+  <si>
+    <t>Canada</t>
+  </si>
+  <si>
     <t>Канада</t>
   </si>
   <si>
-    <t>Canada</t>
-  </si>
-  <si>
-    <t>France</t>
-  </si>
-  <si>
-    <t>Италия</t>
-  </si>
-  <si>
-    <t>Італія</t>
-  </si>
-  <si>
-    <t>Greece</t>
-  </si>
-  <si>
-    <t>Франция</t>
-  </si>
-  <si>
-    <t>Франція</t>
-  </si>
-  <si>
-    <t>Germany</t>
-  </si>
-  <si>
-    <t>Греция</t>
-  </si>
-  <si>
-    <t>Греція</t>
-  </si>
-  <si>
-    <t>Denmark</t>
-  </si>
-  <si>
-    <t>Германия</t>
-  </si>
-  <si>
-    <t>Германія</t>
-  </si>
-  <si>
-    <t>Sweden</t>
-  </si>
-  <si>
-    <t>Дания</t>
-  </si>
-  <si>
-    <t>Данія</t>
-  </si>
-  <si>
-    <t>Norway</t>
-  </si>
-  <si>
-    <t>Швеция</t>
-  </si>
-  <si>
-    <t>Швеція</t>
-  </si>
-  <si>
-    <t>Finland</t>
-  </si>
-  <si>
-    <t>Норвегия</t>
-  </si>
-  <si>
-    <t>Норвегія</t>
-  </si>
-  <si>
-    <t>Spain</t>
-  </si>
-  <si>
-    <t>Финляндия</t>
-  </si>
-  <si>
-    <t>Фінляндія</t>
-  </si>
-  <si>
-    <t>Austria</t>
-  </si>
-  <si>
-    <t>Испания</t>
-  </si>
-  <si>
-    <t>Іспанія</t>
-  </si>
-  <si>
-    <t>Австрия</t>
-  </si>
-  <si>
-    <t>Австрія</t>
-  </si>
-  <si>
     <t>Thailand</t>
   </si>
   <si>
@@ -1221,6 +1221,18 @@
   </si>
   <si>
     <t>Пв-Сх Азія</t>
+  </si>
+  <si>
+    <t>georgia</t>
+  </si>
+  <si>
+    <t>Грузия</t>
+  </si>
+  <si>
+    <t>Georgia</t>
+  </si>
+  <si>
+    <t>Грузія</t>
   </si>
 </sst>
 </file>
@@ -1271,7 +1283,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1298,6 +1310,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3115,9 +3130,6 @@
       <c r="A15" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>251</v>
-      </c>
       <c r="C15" s="2" t="s">
         <v>278</v>
       </c>
@@ -3163,189 +3175,189 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="7" t="s">
         <v>286</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="7" t="s">
         <v>251</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>287</v>
       </c>
       <c r="D18" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="E18" s="2" t="s">
-        <v>287</v>
-      </c>
     </row>
     <row r="19">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="7" t="s">
         <v>289</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="7" t="s">
         <v>251</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>290</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>291</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="7" t="s">
         <v>292</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="7" t="s">
         <v>251</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>293</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>294</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="1" t="s">
+      <c r="A21" s="7" t="s">
         <v>295</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="7" t="s">
         <v>251</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>296</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>297</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="1" t="s">
+      <c r="A22" s="7" t="s">
         <v>298</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="7" t="s">
         <v>251</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>299</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>300</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="1" t="s">
+      <c r="A23" s="7" t="s">
         <v>301</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="7" t="s">
         <v>251</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>302</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>303</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="1" t="s">
+      <c r="A24" s="7" t="s">
         <v>304</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="7" t="s">
         <v>251</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>305</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>306</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="1" t="s">
+      <c r="A25" s="7" t="s">
         <v>307</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" s="7" t="s">
         <v>251</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>308</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>309</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="1" t="s">
+      <c r="A26" s="7" t="s">
         <v>310</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" s="7" t="s">
         <v>251</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>311</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>312</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="1" t="s">
+      <c r="A27" s="7" t="s">
         <v>313</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" s="7" t="s">
         <v>251</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C27" s="9" t="s">
         <v>314</v>
       </c>
-      <c r="D27" s="2" t="s">
-        <v>310</v>
-      </c>
-      <c r="E27" s="2" t="s">
+      <c r="D27" s="9" t="s">
+        <v>313</v>
+      </c>
+      <c r="E27" s="9" t="s">
         <v>315</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="B28" s="1" t="s">
+      <c r="A28" s="7" t="s">
+        <v>316</v>
+      </c>
+      <c r="B28" s="7" t="s">
         <v>259</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C28" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="D28" s="9" t="s">
         <v>316</v>
       </c>
-      <c r="D28" s="2" t="s">
-        <v>313</v>
-      </c>
-      <c r="E28" s="2" t="s">
+      <c r="E28" s="9" t="s">
         <v>317</v>
       </c>
     </row>
@@ -3755,6 +3767,23 @@
       </c>
       <c r="E52" s="1" t="s">
         <v>402</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>406</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SA-2 meduza SA-9 BTC times SA-8 CNBC SA-11 decrypt
</commit_message>
<xml_diff>
--- a/na-service/src/main/resources/data/category/Categories.xlsx
+++ b/na-service/src/main/resources/data/category/Categories.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="407">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="410">
   <si>
     <t>name</t>
   </si>
@@ -732,6 +732,15 @@
   </si>
   <si>
     <t>Медіа</t>
+  </si>
+  <si>
+    <t>bitcoin</t>
+  </si>
+  <si>
+    <t>crypto</t>
+  </si>
+  <si>
+    <t>Bitcoin</t>
   </si>
   <si>
     <t>World</t>
@@ -1863,9 +1872,6 @@
       <c r="A21" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>57</v>
-      </c>
       <c r="C21" s="2" t="s">
         <v>61</v>
       </c>
@@ -2892,6 +2898,23 @@
       </c>
       <c r="E83" s="1" t="s">
         <v>239</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>242</v>
       </c>
     </row>
   </sheetData>
@@ -2928,862 +2951,862 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>243</v>
-      </c>
       <c r="C4" s="2" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="7" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="7" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="7" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="7" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="7" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="7" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="7" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="7" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="7" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="7" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="7" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="7" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>331</v>
+        <v>334</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>331</v>
+        <v>334</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
-        <v>341</v>
+        <v>344</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
-        <v>345</v>
+        <v>348</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>358</v>
+        <v>361</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>359</v>
+        <v>362</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>358</v>
+        <v>361</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="s">
-        <v>360</v>
+        <v>363</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>361</v>
+        <v>364</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>361</v>
+        <v>364</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="s">
-        <v>363</v>
+        <v>366</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="s">
-        <v>366</v>
+        <v>369</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>367</v>
+        <v>370</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>369</v>
+        <v>372</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="B44" s="1" t="s">
         <v>370</v>
       </c>
-      <c r="B44" s="1" t="s">
-        <v>367</v>
-      </c>
       <c r="C44" s="1" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="s">
-        <v>373</v>
+        <v>376</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>367</v>
+        <v>370</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>375</v>
+        <v>378</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>376</v>
+        <v>379</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="s">
-        <v>377</v>
+        <v>380</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>367</v>
+        <v>370</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>378</v>
+        <v>381</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>379</v>
+        <v>382</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>378</v>
+        <v>381</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="s">
-        <v>380</v>
+        <v>383</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>381</v>
+        <v>384</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>382</v>
+        <v>385</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>384</v>
+        <v>387</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="s">
-        <v>385</v>
+        <v>388</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>387</v>
+        <v>390</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="s">
-        <v>389</v>
+        <v>392</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>390</v>
+        <v>393</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>391</v>
+        <v>394</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>392</v>
+        <v>395</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>394</v>
+        <v>397</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>395</v>
+        <v>398</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>394</v>
+        <v>397</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="s">
-        <v>396</v>
+        <v>399</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>397</v>
+        <v>400</v>
       </c>
       <c r="D51" s="7" t="s">
-        <v>398</v>
+        <v>401</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>399</v>
+        <v>402</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>400</v>
+        <v>403</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>401</v>
+        <v>404</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>402</v>
+        <v>405</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="s">
-        <v>403</v>
+        <v>406</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>404</v>
+        <v>407</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>406</v>
+        <v>409</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SA-16 Israel Time SA-17 Forbes on Russian SA-18 Coindesk The Block Crypto
</commit_message>
<xml_diff>
--- a/na-service/src/main/resources/data/category/Categories.xlsx
+++ b/na-service/src/main/resources/data/category/Categories.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="410">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="418">
   <si>
     <t>name</t>
   </si>
@@ -431,30 +431,30 @@
     <t>Theatre</t>
   </si>
   <si>
+    <t>Театр</t>
+  </si>
+  <si>
+    <t>Наука</t>
+  </si>
+  <si>
+    <t>History</t>
+  </si>
+  <si>
     <t>История</t>
   </si>
   <si>
-    <t>History</t>
-  </si>
-  <si>
     <t>Історія</t>
   </si>
   <si>
+    <t>Animals</t>
+  </si>
+  <si>
     <t>Животные</t>
   </si>
   <si>
-    <t>Animals</t>
-  </si>
-  <si>
     <t>Тварини</t>
   </si>
   <si>
-    <t>Театр</t>
-  </si>
-  <si>
-    <t>Наука</t>
-  </si>
-  <si>
     <t>Property</t>
   </si>
   <si>
@@ -743,6 +743,18 @@
     <t>Bitcoin</t>
   </si>
   <si>
+    <t>comedy</t>
+  </si>
+  <si>
+    <t>Комедия</t>
+  </si>
+  <si>
+    <t>Comedy</t>
+  </si>
+  <si>
+    <t>Комедія</t>
+  </si>
+  <si>
     <t>World</t>
   </si>
   <si>
@@ -1242,6 +1254,18 @@
   </si>
   <si>
     <t>Грузія</t>
+  </si>
+  <si>
+    <t>israel</t>
+  </si>
+  <si>
+    <t>Израиль</t>
+  </si>
+  <si>
+    <t>Israel</t>
+  </si>
+  <si>
+    <t>Ізраїль</t>
   </si>
 </sst>
 </file>
@@ -2362,10 +2386,10 @@
         <v>139</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="52">
@@ -2373,44 +2397,44 @@
         <v>114</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>143</v>
+        <v>114</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>87</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>83</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>114</v>
+        <v>144</v>
       </c>
       <c r="E54" s="2" t="s">
         <v>146</v>
@@ -2915,6 +2939,23 @@
       </c>
       <c r="E84" s="1" t="s">
         <v>242</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B85" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="E85" s="7" t="s">
+        <v>246</v>
       </c>
     </row>
   </sheetData>
@@ -2951,862 +2992,879 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="7" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>262</v>
-      </c>
       <c r="C10" s="2" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="7" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="7" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="7" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="7" t="s">
-        <v>298</v>
+        <v>302</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>298</v>
+        <v>302</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="7" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="7" t="s">
-        <v>304</v>
+        <v>308</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>304</v>
+        <v>308</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>306</v>
+        <v>310</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="7" t="s">
-        <v>307</v>
+        <v>311</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>308</v>
+        <v>312</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>307</v>
+        <v>311</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="7" t="s">
-        <v>310</v>
+        <v>314</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>311</v>
+        <v>315</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>310</v>
+        <v>314</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>312</v>
+        <v>316</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="7" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>314</v>
+        <v>318</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>315</v>
+        <v>319</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="7" t="s">
-        <v>316</v>
+        <v>320</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>317</v>
+        <v>321</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>316</v>
+        <v>320</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>318</v>
+        <v>322</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="7" t="s">
-        <v>319</v>
+        <v>323</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>319</v>
+        <v>323</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>322</v>
+        <v>326</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>323</v>
+        <v>327</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>325</v>
+        <v>329</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>326</v>
+        <v>330</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>327</v>
+        <v>331</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>328</v>
+        <v>332</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>329</v>
+        <v>333</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>330</v>
+        <v>334</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>332</v>
+        <v>336</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>333</v>
+        <v>337</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>335</v>
+        <v>339</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>336</v>
+        <v>340</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>337</v>
+        <v>341</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>338</v>
+        <v>342</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>339</v>
+        <v>343</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
-        <v>340</v>
+        <v>344</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>341</v>
+        <v>345</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>342</v>
+        <v>346</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>343</v>
+        <v>347</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
-        <v>344</v>
+        <v>348</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>345</v>
+        <v>349</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>346</v>
+        <v>350</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>347</v>
+        <v>351</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
-        <v>348</v>
+        <v>352</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>349</v>
+        <v>353</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>349</v>
+        <v>353</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="s">
-        <v>351</v>
+        <v>355</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>352</v>
+        <v>356</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>353</v>
+        <v>357</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>352</v>
+        <v>356</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="s">
-        <v>354</v>
+        <v>358</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>355</v>
+        <v>359</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>356</v>
+        <v>360</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>355</v>
+        <v>359</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="s">
-        <v>357</v>
+        <v>361</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>358</v>
+        <v>362</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>359</v>
+        <v>363</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>358</v>
+        <v>362</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="s">
-        <v>360</v>
+        <v>364</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>361</v>
+        <v>365</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>362</v>
+        <v>366</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>361</v>
+        <v>365</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="s">
-        <v>363</v>
+        <v>367</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>364</v>
+        <v>368</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>365</v>
+        <v>369</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>364</v>
+        <v>368</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="s">
-        <v>366</v>
+        <v>370</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>367</v>
+        <v>371</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>367</v>
+        <v>371</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="s">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>371</v>
+        <v>375</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>372</v>
+        <v>376</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>371</v>
+        <v>375</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="s">
-        <v>373</v>
+        <v>377</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>374</v>
+        <v>378</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>375</v>
+        <v>379</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>374</v>
+        <v>378</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="s">
-        <v>376</v>
+        <v>380</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>377</v>
+        <v>381</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>378</v>
+        <v>382</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>379</v>
+        <v>383</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="s">
-        <v>380</v>
+        <v>384</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>381</v>
+        <v>385</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>382</v>
+        <v>386</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>381</v>
+        <v>385</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="s">
-        <v>383</v>
+        <v>387</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>384</v>
+        <v>388</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>385</v>
+        <v>389</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>386</v>
+        <v>390</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>387</v>
+        <v>391</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="s">
-        <v>388</v>
+        <v>392</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>322</v>
+        <v>326</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>390</v>
+        <v>394</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>391</v>
+        <v>395</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="s">
-        <v>392</v>
+        <v>396</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>322</v>
+        <v>326</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>394</v>
+        <v>398</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>395</v>
+        <v>399</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="s">
-        <v>396</v>
+        <v>400</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>322</v>
+        <v>326</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>397</v>
+        <v>401</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>398</v>
+        <v>402</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>397</v>
+        <v>401</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="s">
-        <v>399</v>
+        <v>403</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>322</v>
+        <v>326</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
       <c r="D51" s="7" t="s">
-        <v>401</v>
+        <v>405</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>402</v>
+        <v>406</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="s">
-        <v>322</v>
+        <v>326</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>403</v>
+        <v>407</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>404</v>
+        <v>408</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>405</v>
+        <v>409</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="s">
-        <v>406</v>
+        <v>410</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>407</v>
+        <v>411</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>408</v>
+        <v>412</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>409</v>
+        <v>413</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="E54" s="7" t="s">
+        <v>417</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed admin message notifications
</commit_message>
<xml_diff>
--- a/na-service/src/main/resources/data/category/Categories.xlsx
+++ b/na-service/src/main/resources/data/category/Categories.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="809" uniqueCount="526">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="819" uniqueCount="535">
   <si>
     <t>name</t>
   </si>
@@ -882,6 +882,33 @@
   </si>
   <si>
     <t>Beauty</t>
+  </si>
+  <si>
+    <t>criminal</t>
+  </si>
+  <si>
+    <t>general</t>
+  </si>
+  <si>
+    <t>Криминал</t>
+  </si>
+  <si>
+    <t>Criminal</t>
+  </si>
+  <si>
+    <t>Кримінал</t>
+  </si>
+  <si>
+    <t>incidents</t>
+  </si>
+  <si>
+    <t>Происшествия</t>
+  </si>
+  <si>
+    <t>Incidents</t>
+  </si>
+  <si>
+    <t>Інциденти</t>
   </si>
   <si>
     <t>World</t>
@@ -3483,6 +3510,40 @@
         <v>288</v>
       </c>
     </row>
+    <row r="98">
+      <c r="A98" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="D98" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="E98" s="1" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="E99" s="7" t="s">
+        <v>298</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -3517,1151 +3578,1151 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>290</v>
+        <v>299</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>291</v>
+        <v>300</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>290</v>
+        <v>299</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>292</v>
+        <v>301</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>293</v>
+        <v>302</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>294</v>
+        <v>303</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>293</v>
+        <v>302</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>295</v>
+        <v>304</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>296</v>
+        <v>305</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>293</v>
+        <v>302</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>297</v>
+        <v>306</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>296</v>
+        <v>305</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>297</v>
+        <v>306</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>298</v>
+        <v>307</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>293</v>
+        <v>302</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>299</v>
+        <v>308</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>298</v>
+        <v>307</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>300</v>
+        <v>309</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>301</v>
+        <v>310</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>302</v>
+        <v>311</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>301</v>
+        <v>310</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>303</v>
+        <v>312</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>304</v>
+        <v>313</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>305</v>
+        <v>314</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>306</v>
+        <v>315</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>307</v>
+        <v>316</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>308</v>
+        <v>317</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>309</v>
+        <v>318</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>310</v>
+        <v>319</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>309</v>
+        <v>318</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>310</v>
+        <v>319</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>311</v>
+        <v>320</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>309</v>
+        <v>318</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>312</v>
+        <v>321</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>311</v>
+        <v>320</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>312</v>
+        <v>321</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>313</v>
+        <v>322</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>309</v>
+        <v>318</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>314</v>
+        <v>323</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>313</v>
+        <v>322</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>315</v>
+        <v>324</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>316</v>
+        <v>325</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>317</v>
+        <v>326</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>316</v>
+        <v>325</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>317</v>
+        <v>326</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>318</v>
+        <v>327</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>319</v>
+        <v>328</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>318</v>
+        <v>327</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>320</v>
+        <v>329</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>321</v>
+        <v>330</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>322</v>
+        <v>331</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>321</v>
+        <v>330</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>323</v>
+        <v>332</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>324</v>
+        <v>333</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>301</v>
+        <v>310</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>325</v>
+        <v>334</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>324</v>
+        <v>333</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>326</v>
+        <v>335</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>327</v>
+        <v>336</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>328</v>
+        <v>337</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>327</v>
+        <v>336</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>329</v>
+        <v>338</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>330</v>
+        <v>339</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>304</v>
+        <v>313</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>331</v>
+        <v>340</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>330</v>
+        <v>339</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>332</v>
+        <v>341</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>333</v>
+        <v>342</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>301</v>
+        <v>310</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>334</v>
+        <v>343</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>333</v>
+        <v>342</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>335</v>
+        <v>344</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>336</v>
+        <v>345</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>301</v>
+        <v>310</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>337</v>
+        <v>346</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>336</v>
+        <v>345</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>338</v>
+        <v>347</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>339</v>
+        <v>348</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>301</v>
+        <v>310</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>340</v>
+        <v>349</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>339</v>
+        <v>348</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>341</v>
+        <v>350</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>342</v>
+        <v>351</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>301</v>
+        <v>310</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>343</v>
+        <v>352</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>342</v>
+        <v>351</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>344</v>
+        <v>353</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>345</v>
+        <v>354</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>301</v>
+        <v>310</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>346</v>
+        <v>355</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>345</v>
+        <v>354</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>347</v>
+        <v>356</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>348</v>
+        <v>357</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>301</v>
+        <v>310</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>349</v>
+        <v>358</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>348</v>
+        <v>357</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>351</v>
+        <v>360</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>301</v>
+        <v>310</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>352</v>
+        <v>361</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>351</v>
+        <v>360</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>353</v>
+        <v>362</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>354</v>
+        <v>363</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>301</v>
+        <v>310</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>355</v>
+        <v>364</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>354</v>
+        <v>363</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>356</v>
+        <v>365</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>357</v>
+        <v>366</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>301</v>
+        <v>310</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>358</v>
+        <v>367</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>357</v>
+        <v>366</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>359</v>
+        <v>368</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>360</v>
+        <v>369</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>301</v>
+        <v>310</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>361</v>
+        <v>370</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>360</v>
+        <v>369</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>362</v>
+        <v>371</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>363</v>
+        <v>372</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>301</v>
+        <v>310</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>364</v>
+        <v>373</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>363</v>
+        <v>372</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>365</v>
+        <v>374</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>366</v>
+        <v>375</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>309</v>
+        <v>318</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>367</v>
+        <v>376</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>366</v>
+        <v>375</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>367</v>
+        <v>376</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>368</v>
+        <v>377</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>369</v>
+        <v>378</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>370</v>
+        <v>379</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>368</v>
+        <v>377</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>371</v>
+        <v>380</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>372</v>
+        <v>381</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>324</v>
+        <v>333</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>373</v>
+        <v>382</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>374</v>
+        <v>383</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>375</v>
+        <v>384</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>376</v>
+        <v>385</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>324</v>
+        <v>333</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>377</v>
+        <v>386</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>378</v>
+        <v>387</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>379</v>
+        <v>388</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>380</v>
+        <v>389</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>324</v>
+        <v>333</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>381</v>
+        <v>390</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>382</v>
+        <v>391</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>381</v>
+        <v>390</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>383</v>
+        <v>392</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>324</v>
+        <v>333</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>384</v>
+        <v>393</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>385</v>
+        <v>394</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>386</v>
+        <v>395</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
-        <v>387</v>
+        <v>396</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>324</v>
+        <v>333</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>388</v>
+        <v>397</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>389</v>
+        <v>398</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>390</v>
+        <v>399</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
-        <v>391</v>
+        <v>400</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>324</v>
+        <v>333</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>392</v>
+        <v>401</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>393</v>
+        <v>402</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>394</v>
+        <v>403</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
-        <v>395</v>
+        <v>404</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>368</v>
+        <v>377</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>396</v>
+        <v>405</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>397</v>
+        <v>406</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>396</v>
+        <v>405</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="s">
-        <v>398</v>
+        <v>407</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>368</v>
+        <v>377</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>399</v>
+        <v>408</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>400</v>
+        <v>409</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>399</v>
+        <v>408</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="s">
-        <v>401</v>
+        <v>410</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>368</v>
+        <v>377</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>402</v>
+        <v>411</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>403</v>
+        <v>412</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>402</v>
+        <v>411</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="s">
-        <v>404</v>
+        <v>413</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>368</v>
+        <v>377</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>405</v>
+        <v>414</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>406</v>
+        <v>415</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>405</v>
+        <v>414</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="s">
-        <v>407</v>
+        <v>416</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>368</v>
+        <v>377</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>408</v>
+        <v>417</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>409</v>
+        <v>418</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>408</v>
+        <v>417</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="s">
-        <v>410</v>
+        <v>419</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>368</v>
+        <v>377</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>411</v>
+        <v>420</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>412</v>
+        <v>421</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>411</v>
+        <v>420</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="s">
-        <v>413</v>
+        <v>422</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>313</v>
+        <v>322</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>414</v>
+        <v>423</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>415</v>
+        <v>424</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>414</v>
+        <v>423</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="s">
-        <v>416</v>
+        <v>425</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>417</v>
+        <v>426</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>418</v>
+        <v>427</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>419</v>
+        <v>428</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>418</v>
+        <v>427</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="s">
-        <v>420</v>
+        <v>429</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>417</v>
+        <v>426</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>421</v>
+        <v>430</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>422</v>
+        <v>431</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>421</v>
+        <v>430</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="s">
-        <v>423</v>
+        <v>432</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>417</v>
+        <v>426</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>424</v>
+        <v>433</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>425</v>
+        <v>434</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>426</v>
+        <v>435</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="s">
-        <v>427</v>
+        <v>436</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>417</v>
+        <v>426</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>428</v>
+        <v>437</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>429</v>
+        <v>438</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>428</v>
+        <v>437</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="s">
-        <v>430</v>
+        <v>439</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>431</v>
+        <v>440</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>432</v>
+        <v>441</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>433</v>
+        <v>442</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>434</v>
+        <v>443</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="s">
-        <v>435</v>
+        <v>444</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>369</v>
+        <v>378</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>436</v>
+        <v>445</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>437</v>
+        <v>446</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>438</v>
+        <v>447</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="s">
-        <v>439</v>
+        <v>448</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>369</v>
+        <v>378</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>440</v>
+        <v>449</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>441</v>
+        <v>450</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>442</v>
+        <v>451</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="s">
-        <v>443</v>
+        <v>452</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>369</v>
+        <v>378</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>444</v>
+        <v>453</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>445</v>
+        <v>454</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>444</v>
+        <v>453</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="s">
-        <v>446</v>
+        <v>455</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>369</v>
+        <v>378</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>447</v>
+        <v>456</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>448</v>
+        <v>457</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>449</v>
+        <v>458</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="s">
-        <v>369</v>
+        <v>378</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>293</v>
+        <v>302</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>450</v>
+        <v>459</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>451</v>
+        <v>460</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>452</v>
+        <v>461</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="s">
-        <v>453</v>
+        <v>462</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>301</v>
+        <v>310</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>454</v>
+        <v>463</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>455</v>
+        <v>464</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>456</v>
+        <v>465</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="s">
-        <v>457</v>
+        <v>466</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>321</v>
+        <v>330</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>458</v>
+        <v>467</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>459</v>
+        <v>468</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>460</v>
+        <v>469</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="s">
-        <v>461</v>
+        <v>470</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>305</v>
+        <v>314</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>462</v>
+        <v>471</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>464</v>
+        <v>473</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="s">
-        <v>465</v>
+        <v>474</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>305</v>
+        <v>314</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>466</v>
+        <v>475</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>467</v>
+        <v>476</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>468</v>
+        <v>477</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="s">
-        <v>469</v>
+        <v>478</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>305</v>
+        <v>314</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>470</v>
+        <v>479</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>471</v>
+        <v>480</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>472</v>
+        <v>481</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="s">
-        <v>473</v>
+        <v>482</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>305</v>
+        <v>314</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>474</v>
+        <v>483</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>475</v>
+        <v>484</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>476</v>
+        <v>485</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="s">
-        <v>477</v>
+        <v>486</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>305</v>
+        <v>314</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>478</v>
+        <v>487</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>479</v>
+        <v>488</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>480</v>
+        <v>489</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="s">
-        <v>481</v>
+        <v>490</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>482</v>
+        <v>491</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>483</v>
+        <v>492</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>484</v>
+        <v>493</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>485</v>
+        <v>494</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="s">
-        <v>486</v>
+        <v>495</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>305</v>
+        <v>314</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>487</v>
+        <v>496</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>488</v>
+        <v>497</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>489</v>
+        <v>498</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="s">
-        <v>490</v>
+        <v>499</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>305</v>
+        <v>314</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>491</v>
+        <v>500</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>492</v>
+        <v>501</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>493</v>
+        <v>502</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="s">
-        <v>494</v>
+        <v>503</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>305</v>
+        <v>314</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>495</v>
+        <v>504</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>496</v>
+        <v>505</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>497</v>
+        <v>506</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="s">
-        <v>498</v>
+        <v>507</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>305</v>
+        <v>314</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>499</v>
+        <v>508</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>500</v>
+        <v>509</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>501</v>
+        <v>510</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="s">
-        <v>502</v>
+        <v>511</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>305</v>
+        <v>314</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>503</v>
+        <v>512</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>504</v>
+        <v>513</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>505</v>
+        <v>514</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="s">
-        <v>506</v>
+        <v>515</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>305</v>
+        <v>314</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>507</v>
+        <v>516</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>508</v>
+        <v>517</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>509</v>
+        <v>518</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="s">
-        <v>510</v>
+        <v>519</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>305</v>
+        <v>314</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>511</v>
+        <v>520</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>512</v>
+        <v>521</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>513</v>
+        <v>522</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="s">
-        <v>514</v>
+        <v>523</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>305</v>
+        <v>314</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>515</v>
+        <v>524</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>516</v>
+        <v>525</v>
       </c>
       <c r="E68" s="7" t="s">
-        <v>517</v>
+        <v>526</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="s">
-        <v>518</v>
+        <v>527</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>305</v>
+        <v>314</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>519</v>
+        <v>528</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>520</v>
+        <v>529</v>
       </c>
       <c r="E69" s="7" t="s">
-        <v>521</v>
+        <v>530</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="s">
-        <v>522</v>
+        <v>531</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>305</v>
+        <v>314</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>523</v>
+        <v>532</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>524</v>
+        <v>533</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>525</v>
+        <v>534</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
removed source page name
</commit_message>
<xml_diff>
--- a/na-service/src/main/resources/data/category/Categories.xlsx
+++ b/na-service/src/main/resources/data/category/Categories.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="819" uniqueCount="535">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1073" uniqueCount="707">
   <si>
     <t>name</t>
   </si>
@@ -911,6 +911,42 @@
     <t>Інциденти</t>
   </si>
   <si>
+    <t>faith</t>
+  </si>
+  <si>
+    <t>Вера</t>
+  </si>
+  <si>
+    <t>Faith</t>
+  </si>
+  <si>
+    <t>Віра</t>
+  </si>
+  <si>
+    <t>islam</t>
+  </si>
+  <si>
+    <t>Ислам</t>
+  </si>
+  <si>
+    <t>Islam</t>
+  </si>
+  <si>
+    <t>Іслам</t>
+  </si>
+  <si>
+    <t>corruption</t>
+  </si>
+  <si>
+    <t>Коррупция</t>
+  </si>
+  <si>
+    <t>Corruption</t>
+  </si>
+  <si>
+    <t>Корупція</t>
+  </si>
+  <si>
     <t>World</t>
   </si>
   <si>
@@ -1424,6 +1460,30 @@
     <t>Ізраїль</t>
   </si>
   <si>
+    <t>iran</t>
+  </si>
+  <si>
+    <t>Иран</t>
+  </si>
+  <si>
+    <t>Iran</t>
+  </si>
+  <si>
+    <t>Іран</t>
+  </si>
+  <si>
+    <t>irak</t>
+  </si>
+  <si>
+    <t>Ирак</t>
+  </si>
+  <si>
+    <t>Iraq</t>
+  </si>
+  <si>
+    <t>Ірак</t>
+  </si>
+  <si>
     <t>lithuania</t>
   </si>
   <si>
@@ -1617,13 +1677,469 @@
   </si>
   <si>
     <t>Турція</t>
+  </si>
+  <si>
+    <t>donetsk</t>
+  </si>
+  <si>
+    <t>ukraine</t>
+  </si>
+  <si>
+    <t>Донецк</t>
+  </si>
+  <si>
+    <t>Donetsk</t>
+  </si>
+  <si>
+    <t>Донецьк</t>
+  </si>
+  <si>
+    <t>abkhazia</t>
+  </si>
+  <si>
+    <t>Абхазия</t>
+  </si>
+  <si>
+    <t>Abkhazia</t>
+  </si>
+  <si>
+    <t>Абхазія</t>
+  </si>
+  <si>
+    <t>bilatserkva</t>
+  </si>
+  <si>
+    <t>Белая Церковь</t>
+  </si>
+  <si>
+    <t>Біла Церква</t>
+  </si>
+  <si>
+    <t>afgan</t>
+  </si>
+  <si>
+    <t>Афганистан</t>
+  </si>
+  <si>
+    <t>Afganistan</t>
+  </si>
+  <si>
+    <t>Афганістан</t>
+  </si>
+  <si>
+    <t>zhytomir</t>
+  </si>
+  <si>
+    <t>Житомир</t>
+  </si>
+  <si>
+    <t>zakarpaty</t>
+  </si>
+  <si>
+    <t>Закарпатье</t>
+  </si>
+  <si>
+    <t>Закарпаття</t>
+  </si>
+  <si>
+    <t>ivanofrankovsk</t>
+  </si>
+  <si>
+    <t>Ивано-Франковск</t>
+  </si>
+  <si>
+    <t>Івано-Франківськ</t>
+  </si>
+  <si>
+    <t>izum</t>
+  </si>
+  <si>
+    <t>Изюм</t>
+  </si>
+  <si>
+    <t>Ізюм</t>
+  </si>
+  <si>
+    <t>irpin</t>
+  </si>
+  <si>
+    <t>Ирпень</t>
+  </si>
+  <si>
+    <t>Ірпінь</t>
+  </si>
+  <si>
+    <t>ireland</t>
+  </si>
+  <si>
+    <t>Ирландия</t>
+  </si>
+  <si>
+    <t>Ireland</t>
+  </si>
+  <si>
+    <t>Ірландія</t>
+  </si>
+  <si>
+    <t>kazah</t>
+  </si>
+  <si>
+    <t>Казахстан</t>
+  </si>
+  <si>
+    <t>kerch</t>
+  </si>
+  <si>
+    <t>Керчь</t>
+  </si>
+  <si>
+    <t>Керч</t>
+  </si>
+  <si>
+    <t>kropivnitskiy</t>
+  </si>
+  <si>
+    <t>Кропивныцкий</t>
+  </si>
+  <si>
+    <t>Кропівницький</t>
+  </si>
+  <si>
+    <t>kremen</t>
+  </si>
+  <si>
+    <t>Кременчуг</t>
+  </si>
+  <si>
+    <t>Кременчук</t>
+  </si>
+  <si>
+    <t>krivij-rig</t>
+  </si>
+  <si>
+    <t>Кривой Рог</t>
+  </si>
+  <si>
+    <t>Кривий Ріг</t>
+  </si>
+  <si>
+    <t>kramatorsk</t>
+  </si>
+  <si>
+    <t>Краматорск</t>
+  </si>
+  <si>
+    <t>Краматорськ</t>
+  </si>
+  <si>
+    <t>lugansk</t>
+  </si>
+  <si>
+    <t>Луганск</t>
+  </si>
+  <si>
+    <t>Луганськ</t>
+  </si>
+  <si>
+    <t>mariupol</t>
+  </si>
+  <si>
+    <t>Мариуполь</t>
+  </si>
+  <si>
+    <t>Маріуполь</t>
+  </si>
+  <si>
+    <t>indonesia</t>
+  </si>
+  <si>
+    <t>Индонезия</t>
+  </si>
+  <si>
+    <t>Indonesia</t>
+  </si>
+  <si>
+    <t>Індонезія</t>
+  </si>
+  <si>
+    <t>malaysia</t>
+  </si>
+  <si>
+    <t>Малазия</t>
+  </si>
+  <si>
+    <t>Malaysia</t>
+  </si>
+  <si>
+    <t>Малазія</t>
+  </si>
+  <si>
+    <t>macedonia</t>
+  </si>
+  <si>
+    <t>Македония</t>
+  </si>
+  <si>
+    <t>Macedonia</t>
+  </si>
+  <si>
+    <t>Македонія</t>
+  </si>
+  <si>
+    <t>lutsk</t>
+  </si>
+  <si>
+    <t>Луцк</t>
+  </si>
+  <si>
+    <t>Луцьк</t>
+  </si>
+  <si>
+    <t>mongolia</t>
+  </si>
+  <si>
+    <t>Монголия</t>
+  </si>
+  <si>
+    <t>Mongolia</t>
+  </si>
+  <si>
+    <t>Монголія</t>
+  </si>
+  <si>
+    <t>s-korea</t>
+  </si>
+  <si>
+    <t>Южная Корея</t>
+  </si>
+  <si>
+    <t>SouthKorea</t>
+  </si>
+  <si>
+    <t>Південна Корея</t>
+  </si>
+  <si>
+    <t>n-korea</t>
+  </si>
+  <si>
+    <t>Северная Корея</t>
+  </si>
+  <si>
+    <t>NorthKorea</t>
+  </si>
+  <si>
+    <t>Північна Корея</t>
+  </si>
+  <si>
+    <t>poltava</t>
+  </si>
+  <si>
+    <t>Полтава</t>
+  </si>
+  <si>
+    <t>romania</t>
+  </si>
+  <si>
+    <t>Румыния</t>
+  </si>
+  <si>
+    <t>Romania</t>
+  </si>
+  <si>
+    <t>Румунія</t>
+  </si>
+  <si>
+    <t>siriya</t>
+  </si>
+  <si>
+    <t>Сирия</t>
+  </si>
+  <si>
+    <t>Siria</t>
+  </si>
+  <si>
+    <t>Сірія</t>
+  </si>
+  <si>
+    <t>serbia</t>
+  </si>
+  <si>
+    <t>Сербия</t>
+  </si>
+  <si>
+    <t>Serbia</t>
+  </si>
+  <si>
+    <t>Сербія</t>
+  </si>
+  <si>
+    <t>crimea</t>
+  </si>
+  <si>
+    <t>Крым</t>
+  </si>
+  <si>
+    <t>Crimea</t>
+  </si>
+  <si>
+    <t>Крим</t>
+  </si>
+  <si>
+    <t>slovakia</t>
+  </si>
+  <si>
+    <t>Словакия</t>
+  </si>
+  <si>
+    <t>Slovakia</t>
+  </si>
+  <si>
+    <t>Словакія</t>
+  </si>
+  <si>
+    <t>slovenia</t>
+  </si>
+  <si>
+    <t>Словения</t>
+  </si>
+  <si>
+    <t>Slovenia</t>
+  </si>
+  <si>
+    <t>Словенія</t>
+  </si>
+  <si>
+    <t>sumi</t>
+  </si>
+  <si>
+    <t>Суммы</t>
+  </si>
+  <si>
+    <t>Суми</t>
+  </si>
+  <si>
+    <t>ternopol</t>
+  </si>
+  <si>
+    <t>Тернополь</t>
+  </si>
+  <si>
+    <t>Тернопіль</t>
+  </si>
+  <si>
+    <t>turkmenistan</t>
+  </si>
+  <si>
+    <t>Туркменистан</t>
+  </si>
+  <si>
+    <t>Turkmenistan</t>
+  </si>
+  <si>
+    <t>Туркменістан</t>
+  </si>
+  <si>
+    <t>uzbekistan</t>
+  </si>
+  <si>
+    <t>Узбекистан</t>
+  </si>
+  <si>
+    <t>Uzbekistan</t>
+  </si>
+  <si>
+    <t>Узбекістан</t>
+  </si>
+  <si>
+    <t>uman</t>
+  </si>
+  <si>
+    <t>Умань</t>
+  </si>
+  <si>
+    <t>kherson</t>
+  </si>
+  <si>
+    <t>Херсон</t>
+  </si>
+  <si>
+    <t>khmelnitskij</t>
+  </si>
+  <si>
+    <t>Хмельницкий</t>
+  </si>
+  <si>
+    <t>Хмельницький</t>
+  </si>
+  <si>
+    <t>cherkasi</t>
+  </si>
+  <si>
+    <t>Черкассы</t>
+  </si>
+  <si>
+    <t>Черкаси</t>
+  </si>
+  <si>
+    <t>4ernivtsi</t>
+  </si>
+  <si>
+    <t>Черновцы</t>
+  </si>
+  <si>
+    <t>Чернівці</t>
+  </si>
+  <si>
+    <t>4ernigiv</t>
+  </si>
+  <si>
+    <t>Чернигов</t>
+  </si>
+  <si>
+    <t>Чернігів</t>
+  </si>
+  <si>
+    <t>chornobil</t>
+  </si>
+  <si>
+    <t>Чернобыль</t>
+  </si>
+  <si>
+    <t>Chornobyl</t>
+  </si>
+  <si>
+    <t>Чорнобиль</t>
+  </si>
+  <si>
+    <t>switzerland</t>
+  </si>
+  <si>
+    <t>Швейцария</t>
+  </si>
+  <si>
+    <t>Switzerland</t>
+  </si>
+  <si>
+    <t>Швейцарія</t>
+  </si>
+  <si>
+    <t>srilanka</t>
+  </si>
+  <si>
+    <t>Шри-Ланка</t>
+  </si>
+  <si>
+    <t>Sri-Lanka</t>
+  </si>
+  <si>
+    <t>Шрі-Ланка</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -1643,6 +2159,11 @@
       <name val="Arial"/>
     </font>
     <font/>
+    <font>
+      <u/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1664,7 +2185,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1686,11 +2207,17 @@
     <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3358,10 +3885,10 @@
       </c>
     </row>
     <row r="89">
-      <c r="A89" s="7" t="s">
+      <c r="A89" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="B89" s="7" t="s">
+      <c r="B89" s="1" t="s">
         <v>259</v>
       </c>
       <c r="C89" s="1" t="s">
@@ -3370,15 +3897,15 @@
       <c r="D89" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="E89" s="7" t="s">
+      <c r="E89" s="1" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="90">
-      <c r="A90" s="7" t="s">
+      <c r="A90" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="B90" s="7" t="s">
+      <c r="B90" s="1" t="s">
         <v>264</v>
       </c>
       <c r="C90" s="1" t="s">
@@ -3438,7 +3965,7 @@
       <c r="D93" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="E93" s="7" t="s">
+      <c r="E93" s="1" t="s">
         <v>275</v>
       </c>
     </row>
@@ -3540,8 +4067,56 @@
       <c r="D99" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="E99" s="7" t="s">
+      <c r="E99" s="1" t="s">
         <v>298</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="D100" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="E100" s="1" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="D101" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="E101" s="1" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="D102" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="E102" s="1" t="s">
+        <v>310</v>
       </c>
     </row>
   </sheetData>
@@ -3578,1151 +4153,1967 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>299</v>
+        <v>311</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>300</v>
+        <v>312</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>299</v>
+        <v>311</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>301</v>
+        <v>313</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>302</v>
+        <v>314</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>303</v>
+        <v>315</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>302</v>
+        <v>314</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>304</v>
+        <v>316</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>305</v>
+        <v>317</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>302</v>
+        <v>314</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>306</v>
+        <v>318</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>305</v>
+        <v>317</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>306</v>
+        <v>318</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>307</v>
+        <v>319</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>302</v>
+        <v>314</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>308</v>
+        <v>320</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>307</v>
+        <v>319</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>309</v>
+        <v>321</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>310</v>
+        <v>322</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>311</v>
+        <v>323</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>310</v>
+        <v>322</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>312</v>
+        <v>324</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>313</v>
+        <v>325</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>315</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>316</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>317</v>
+        <v>326</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>327</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>328</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>329</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>318</v>
+        <v>330</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>319</v>
+        <v>331</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>318</v>
+        <v>330</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>319</v>
+        <v>331</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>320</v>
+        <v>332</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>318</v>
+        <v>330</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>321</v>
+        <v>333</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>320</v>
+        <v>332</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>321</v>
+        <v>333</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>322</v>
+        <v>334</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>318</v>
+        <v>330</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>323</v>
+        <v>335</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>322</v>
+        <v>334</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>324</v>
+        <v>336</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>325</v>
+        <v>337</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>326</v>
+        <v>338</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>325</v>
+        <v>337</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>326</v>
+        <v>338</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>327</v>
+        <v>339</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>328</v>
+        <v>340</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>327</v>
+        <v>339</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>329</v>
+        <v>341</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>330</v>
+        <v>342</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>331</v>
+        <v>343</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>330</v>
+        <v>342</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>332</v>
+        <v>344</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>333</v>
+        <v>345</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>310</v>
+        <v>322</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>334</v>
+        <v>346</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>333</v>
+        <v>345</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>335</v>
+        <v>347</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>336</v>
+        <v>348</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>337</v>
+        <v>349</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>336</v>
+        <v>348</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>338</v>
+        <v>350</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>339</v>
+        <v>351</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>313</v>
+        <v>325</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>340</v>
+        <v>352</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>339</v>
+        <v>351</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>341</v>
+        <v>353</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>342</v>
+        <v>354</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>310</v>
+        <v>322</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>343</v>
+        <v>355</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>342</v>
+        <v>354</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>344</v>
+        <v>356</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>345</v>
+        <v>357</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>310</v>
+        <v>322</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>346</v>
+        <v>358</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>345</v>
+        <v>357</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>347</v>
+        <v>359</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>348</v>
+        <v>360</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>310</v>
+        <v>322</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>349</v>
+        <v>361</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>348</v>
+        <v>360</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>350</v>
+        <v>362</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>351</v>
+        <v>363</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>310</v>
+        <v>322</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>352</v>
+        <v>364</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>351</v>
+        <v>363</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>353</v>
+        <v>365</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>354</v>
+        <v>366</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>310</v>
+        <v>322</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>355</v>
+        <v>367</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>354</v>
+        <v>366</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>356</v>
+        <v>368</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>357</v>
+        <v>369</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>310</v>
+        <v>322</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>358</v>
+        <v>370</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>357</v>
+        <v>369</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>359</v>
+        <v>371</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>360</v>
+        <v>372</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>310</v>
+        <v>322</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>361</v>
+        <v>373</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>360</v>
+        <v>372</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>362</v>
+        <v>374</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>363</v>
+        <v>375</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>310</v>
+        <v>322</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>364</v>
+        <v>376</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>363</v>
+        <v>375</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>365</v>
+        <v>377</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>366</v>
+        <v>378</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>310</v>
+        <v>322</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>367</v>
+        <v>379</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>366</v>
+        <v>378</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>368</v>
+        <v>380</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>369</v>
+        <v>381</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>310</v>
+        <v>322</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>370</v>
+        <v>382</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>369</v>
+        <v>381</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>371</v>
+        <v>383</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>372</v>
+        <v>384</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>310</v>
+        <v>322</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>373</v>
+        <v>385</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>372</v>
+        <v>384</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>374</v>
+        <v>386</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>375</v>
+        <v>387</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>318</v>
+        <v>330</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>376</v>
+        <v>388</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>375</v>
+        <v>387</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>376</v>
+        <v>388</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>377</v>
+        <v>389</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>378</v>
+        <v>390</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>379</v>
+        <v>391</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>377</v>
+        <v>389</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>380</v>
+        <v>392</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>381</v>
+        <v>393</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>333</v>
+        <v>345</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>382</v>
+        <v>394</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>383</v>
+        <v>395</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>384</v>
+        <v>396</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>385</v>
+        <v>397</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>333</v>
+        <v>345</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>386</v>
+        <v>398</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>387</v>
+        <v>399</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>388</v>
+        <v>400</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>389</v>
+        <v>401</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>333</v>
+        <v>345</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>390</v>
+        <v>402</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>391</v>
+        <v>403</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>390</v>
+        <v>402</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>392</v>
+        <v>404</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>333</v>
+        <v>345</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>393</v>
+        <v>405</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>394</v>
+        <v>406</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>395</v>
+        <v>407</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
-        <v>396</v>
+        <v>408</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>333</v>
+        <v>345</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>397</v>
+        <v>409</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>398</v>
+        <v>410</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>399</v>
+        <v>411</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
-        <v>400</v>
+        <v>412</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>333</v>
+        <v>345</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>401</v>
+        <v>413</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>402</v>
+        <v>414</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>403</v>
+        <v>415</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
-        <v>404</v>
+        <v>416</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>377</v>
+        <v>389</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>405</v>
+        <v>417</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>406</v>
+        <v>418</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>405</v>
+        <v>417</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="s">
-        <v>407</v>
+        <v>419</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>377</v>
+        <v>389</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>408</v>
+        <v>420</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>409</v>
+        <v>421</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>408</v>
+        <v>420</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="s">
-        <v>410</v>
+        <v>422</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>377</v>
+        <v>389</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>411</v>
+        <v>423</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>412</v>
+        <v>424</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>411</v>
+        <v>423</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="s">
-        <v>413</v>
+        <v>425</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>377</v>
+        <v>389</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>414</v>
+        <v>426</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>415</v>
+        <v>427</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>414</v>
+        <v>426</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="s">
-        <v>416</v>
+        <v>428</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>377</v>
+        <v>389</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>417</v>
+        <v>429</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>418</v>
+        <v>430</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>417</v>
+        <v>429</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="s">
-        <v>419</v>
+        <v>431</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>377</v>
+        <v>389</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>420</v>
+        <v>432</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>421</v>
+        <v>433</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>420</v>
+        <v>432</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="s">
-        <v>422</v>
+        <v>434</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>322</v>
+        <v>334</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>423</v>
+        <v>435</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>424</v>
+        <v>436</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>423</v>
+        <v>435</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="s">
-        <v>425</v>
+        <v>437</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>426</v>
+        <v>438</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>427</v>
+        <v>439</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>428</v>
+        <v>440</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>427</v>
+        <v>439</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="s">
-        <v>429</v>
+        <v>441</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>426</v>
+        <v>438</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>430</v>
+        <v>442</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>431</v>
+        <v>443</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>430</v>
+        <v>442</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="s">
-        <v>432</v>
+        <v>444</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>426</v>
+        <v>438</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>433</v>
+        <v>445</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>434</v>
+        <v>446</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>435</v>
+        <v>447</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="s">
-        <v>436</v>
+        <v>448</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>426</v>
+        <v>438</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>437</v>
+        <v>449</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>438</v>
+        <v>450</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>437</v>
+        <v>449</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="s">
-        <v>439</v>
+        <v>451</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>440</v>
+        <v>452</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>441</v>
+        <v>453</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>442</v>
+        <v>454</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>443</v>
+        <v>455</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="s">
-        <v>444</v>
+        <v>456</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>378</v>
+        <v>390</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>445</v>
+        <v>457</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>446</v>
+        <v>458</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>447</v>
+        <v>459</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="s">
-        <v>448</v>
+        <v>460</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>378</v>
+        <v>390</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>449</v>
+        <v>461</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>450</v>
+        <v>462</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>451</v>
+        <v>463</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="s">
-        <v>452</v>
+        <v>464</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>378</v>
+        <v>390</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>453</v>
+        <v>465</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>454</v>
+        <v>466</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>453</v>
+        <v>465</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="s">
-        <v>455</v>
+        <v>467</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>378</v>
+        <v>390</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>456</v>
+        <v>468</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>457</v>
+        <v>469</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>458</v>
+        <v>470</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="s">
-        <v>378</v>
+        <v>390</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>302</v>
+        <v>314</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>459</v>
+        <v>471</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>460</v>
+        <v>472</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>461</v>
+        <v>473</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="s">
-        <v>462</v>
+        <v>474</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>310</v>
+        <v>322</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>463</v>
+        <v>475</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>464</v>
+        <v>476</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>465</v>
+        <v>477</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="s">
-        <v>466</v>
+        <v>478</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>330</v>
+        <v>342</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>467</v>
+        <v>479</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>468</v>
+        <v>480</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>469</v>
+        <v>481</v>
       </c>
     </row>
     <row r="55">
-      <c r="A55" s="1" t="s">
-        <v>470</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>471</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>472</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>473</v>
+      <c r="A55" s="8" t="s">
+        <v>482</v>
+      </c>
+      <c r="B55" s="8" t="s">
+        <v>342</v>
+      </c>
+      <c r="C55" s="8" t="s">
+        <v>483</v>
+      </c>
+      <c r="D55" s="8" t="s">
+        <v>484</v>
+      </c>
+      <c r="E55" s="8" t="s">
+        <v>485</v>
       </c>
     </row>
     <row r="56">
-      <c r="A56" s="1" t="s">
-        <v>474</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>475</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>476</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>477</v>
+      <c r="A56" s="8" t="s">
+        <v>486</v>
+      </c>
+      <c r="B56" s="8" t="s">
+        <v>342</v>
+      </c>
+      <c r="C56" s="8" t="s">
+        <v>487</v>
+      </c>
+      <c r="D56" s="8" t="s">
+        <v>488</v>
+      </c>
+      <c r="E56" s="8" t="s">
+        <v>489</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="s">
-        <v>478</v>
+        <v>490</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>314</v>
+        <v>326</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>479</v>
+        <v>491</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>480</v>
+        <v>492</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>481</v>
+        <v>493</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="s">
-        <v>482</v>
+        <v>494</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>314</v>
+        <v>326</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>483</v>
+        <v>495</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>484</v>
+        <v>496</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>485</v>
+        <v>497</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="s">
-        <v>486</v>
+        <v>498</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>314</v>
+        <v>326</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>487</v>
+        <v>499</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>488</v>
+        <v>500</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>489</v>
+        <v>501</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="s">
-        <v>490</v>
+        <v>502</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>491</v>
+        <v>326</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>492</v>
+        <v>503</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>493</v>
+        <v>504</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>494</v>
+        <v>505</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="s">
-        <v>495</v>
+        <v>506</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>314</v>
+        <v>326</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>496</v>
+        <v>507</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>497</v>
+        <v>508</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>498</v>
+        <v>509</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="s">
-        <v>499</v>
+        <v>510</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>314</v>
+        <v>511</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>500</v>
+        <v>512</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>501</v>
+        <v>513</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>502</v>
+        <v>514</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="s">
-        <v>503</v>
+        <v>515</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>314</v>
+        <v>326</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>504</v>
+        <v>516</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>505</v>
+        <v>517</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>506</v>
+        <v>518</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="s">
-        <v>507</v>
+        <v>519</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>314</v>
+        <v>326</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>508</v>
+        <v>520</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>509</v>
+        <v>521</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>510</v>
+        <v>522</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="s">
-        <v>511</v>
+        <v>523</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>314</v>
+        <v>326</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>512</v>
+        <v>524</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>513</v>
+        <v>525</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>514</v>
+        <v>526</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="s">
-        <v>515</v>
+        <v>527</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>314</v>
+        <v>326</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>516</v>
+        <v>528</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>517</v>
+        <v>529</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>518</v>
+        <v>530</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="s">
-        <v>519</v>
+        <v>531</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>314</v>
+        <v>326</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>520</v>
+        <v>532</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>521</v>
+        <v>533</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>522</v>
+        <v>534</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="s">
-        <v>523</v>
+        <v>535</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>314</v>
+        <v>326</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>524</v>
+        <v>536</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>525</v>
-      </c>
-      <c r="E68" s="7" t="s">
-        <v>526</v>
+        <v>537</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>538</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="s">
-        <v>527</v>
+        <v>539</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>314</v>
+        <v>326</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>528</v>
+        <v>540</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>529</v>
-      </c>
-      <c r="E69" s="7" t="s">
-        <v>530</v>
+        <v>541</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>542</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="s">
-        <v>531</v>
+        <v>543</v>
       </c>
       <c r="B70" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>544</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>545</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>548</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>549</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="1" t="s">
+        <v>551</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>552</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>553</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="1" t="s">
+        <v>555</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>558</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="1" t="s">
+        <v>560</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>561</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>562</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="1" t="s">
+        <v>564</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>565</v>
+      </c>
+      <c r="D75" s="8" t="s">
+        <v>566</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="B76" s="1" t="s">
         <v>314</v>
       </c>
-      <c r="C70" s="1" t="s">
-        <v>532</v>
-      </c>
-      <c r="D70" s="1" t="s">
-        <v>533</v>
-      </c>
-      <c r="E70" s="1" t="s">
-        <v>534</v>
+      <c r="C76" s="1" t="s">
+        <v>568</v>
+      </c>
+      <c r="D76" s="8" t="s">
+        <v>569</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="1" t="s">
+        <v>571</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>572</v>
+      </c>
+      <c r="D77" s="8" t="s">
+        <v>572</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="1" t="s">
+        <v>573</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>574</v>
+      </c>
+      <c r="D78" s="8" t="s">
+        <v>575</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="1" t="s">
+        <v>576</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>577</v>
+      </c>
+      <c r="D79" s="8" t="s">
+        <v>578</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="1" t="s">
+        <v>579</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>580</v>
+      </c>
+      <c r="D80" s="8" t="s">
+        <v>581</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="1" t="s">
+        <v>582</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>583</v>
+      </c>
+      <c r="D81" s="8" t="s">
+        <v>584</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="1" t="s">
+        <v>585</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>586</v>
+      </c>
+      <c r="D82" s="8" t="s">
+        <v>587</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="1" t="s">
+        <v>589</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>590</v>
+      </c>
+      <c r="D83" s="8" t="s">
+        <v>590</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="1" t="s">
+        <v>591</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>592</v>
+      </c>
+      <c r="D84" s="8" t="s">
+        <v>593</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="1" t="s">
+        <v>594</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>595</v>
+      </c>
+      <c r="D85" s="8" t="s">
+        <v>596</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="1" t="s">
+        <v>597</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>598</v>
+      </c>
+      <c r="D86" s="8" t="s">
+        <v>599</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="9" t="s">
+        <v>600</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="D87" s="8" t="s">
+        <v>602</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="6" t="s">
+        <v>603</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>604</v>
+      </c>
+      <c r="D88" s="8" t="s">
+        <v>605</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="6" t="s">
+        <v>606</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>607</v>
+      </c>
+      <c r="D89" s="8" t="s">
+        <v>608</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="1" t="s">
+        <v>609</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>610</v>
+      </c>
+      <c r="D90" s="8" t="s">
+        <v>611</v>
+      </c>
+      <c r="E90" s="1" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="1" t="s">
+        <v>612</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>613</v>
+      </c>
+      <c r="D91" s="8" t="s">
+        <v>614</v>
+      </c>
+      <c r="E91" s="1" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="1" t="s">
+        <v>616</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>617</v>
+      </c>
+      <c r="D92" s="8" t="s">
+        <v>618</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="1" t="s">
+        <v>620</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>621</v>
+      </c>
+      <c r="D93" s="8" t="s">
+        <v>622</v>
+      </c>
+      <c r="E93" s="1" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="1" t="s">
+        <v>624</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>625</v>
+      </c>
+      <c r="D94" s="8" t="s">
+        <v>626</v>
+      </c>
+      <c r="E94" s="1" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="1" t="s">
+        <v>627</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>628</v>
+      </c>
+      <c r="D95" s="8" t="s">
+        <v>629</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="1" t="s">
+        <v>631</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>632</v>
+      </c>
+      <c r="D96" s="8" t="s">
+        <v>633</v>
+      </c>
+      <c r="E96" s="1" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="1" t="s">
+        <v>635</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>636</v>
+      </c>
+      <c r="D97" s="8" t="s">
+        <v>637</v>
+      </c>
+      <c r="E97" s="1" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="1" t="s">
+        <v>639</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>640</v>
+      </c>
+      <c r="D98" s="8" t="s">
+        <v>640</v>
+      </c>
+      <c r="E98" s="1" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="1" t="s">
+        <v>641</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>642</v>
+      </c>
+      <c r="D99" s="8" t="s">
+        <v>643</v>
+      </c>
+      <c r="E99" s="1" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="1" t="s">
+        <v>645</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>646</v>
+      </c>
+      <c r="D100" s="8" t="s">
+        <v>647</v>
+      </c>
+      <c r="E100" s="8" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="1" t="s">
+        <v>649</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>650</v>
+      </c>
+      <c r="D101" s="8" t="s">
+        <v>651</v>
+      </c>
+      <c r="E101" s="1" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="1" t="s">
+        <v>653</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>654</v>
+      </c>
+      <c r="D102" s="8" t="s">
+        <v>655</v>
+      </c>
+      <c r="E102" s="1" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="1" t="s">
+        <v>657</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>658</v>
+      </c>
+      <c r="D103" s="8" t="s">
+        <v>659</v>
+      </c>
+      <c r="E103" s="1" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="6" t="s">
+        <v>661</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>662</v>
+      </c>
+      <c r="D104" s="8" t="s">
+        <v>663</v>
+      </c>
+      <c r="E104" s="1" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="1" t="s">
+        <v>665</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>666</v>
+      </c>
+      <c r="D105" s="8" t="s">
+        <v>667</v>
+      </c>
+      <c r="E105" s="1" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="6" t="s">
+        <v>668</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>669</v>
+      </c>
+      <c r="D106" s="8" t="s">
+        <v>670</v>
+      </c>
+      <c r="E106" s="1" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="6" t="s">
+        <v>671</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>672</v>
+      </c>
+      <c r="D107" s="8" t="s">
+        <v>673</v>
+      </c>
+      <c r="E107" s="8" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="1" t="s">
+        <v>675</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>676</v>
+      </c>
+      <c r="D108" s="8" t="s">
+        <v>677</v>
+      </c>
+      <c r="E108" s="1" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="1" t="s">
+        <v>679</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>680</v>
+      </c>
+      <c r="D109" s="8" t="s">
+        <v>680</v>
+      </c>
+      <c r="E109" s="1" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="6" t="s">
+        <v>681</v>
+      </c>
+      <c r="B110" s="8" t="s">
+        <v>556</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>682</v>
+      </c>
+      <c r="D110" s="8" t="s">
+        <v>682</v>
+      </c>
+      <c r="E110" s="1" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="10" t="s">
+        <v>683</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>684</v>
+      </c>
+      <c r="D111" s="8" t="s">
+        <v>685</v>
+      </c>
+      <c r="E111" s="1" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>495</v>
+      </c>
+      <c r="D112" s="8" t="s">
+        <v>496</v>
+      </c>
+      <c r="E112" s="1" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" s="10" t="s">
+        <v>686</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>687</v>
+      </c>
+      <c r="D113" s="8" t="s">
+        <v>688</v>
+      </c>
+      <c r="E113" s="1" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="6" t="s">
+        <v>689</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>690</v>
+      </c>
+      <c r="D114" s="8" t="s">
+        <v>691</v>
+      </c>
+      <c r="E114" s="1" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="6" t="s">
+        <v>692</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>693</v>
+      </c>
+      <c r="D115" s="8" t="s">
+        <v>694</v>
+      </c>
+      <c r="E115" s="1" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="6" t="s">
+        <v>695</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>696</v>
+      </c>
+      <c r="D116" s="8" t="s">
+        <v>697</v>
+      </c>
+      <c r="E116" s="1" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="1" t="s">
+        <v>699</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>700</v>
+      </c>
+      <c r="D117" s="8" t="s">
+        <v>701</v>
+      </c>
+      <c r="E117" s="1" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="1" t="s">
+        <v>703</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>704</v>
+      </c>
+      <c r="D118" s="8" t="s">
+        <v>705</v>
+      </c>
+      <c r="E118" s="1" t="s">
+        <v>706</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added usage of source page parser tracker
</commit_message>
<xml_diff>
--- a/na-service/src/main/resources/data/category/Categories.xlsx
+++ b/na-service/src/main/resources/data/category/Categories.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1068" uniqueCount="707">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1138" uniqueCount="757">
   <si>
     <t>name</t>
   </si>
@@ -947,6 +947,30 @@
     <t>Корупція</t>
   </si>
   <si>
+    <t>opinion</t>
+  </si>
+  <si>
+    <t>Мнение</t>
+  </si>
+  <si>
+    <t>Opinion</t>
+  </si>
+  <si>
+    <t>Думка</t>
+  </si>
+  <si>
+    <t>home-lifestyle</t>
+  </si>
+  <si>
+    <t>Дом</t>
+  </si>
+  <si>
+    <t>Home</t>
+  </si>
+  <si>
+    <t>Вдома</t>
+  </si>
+  <si>
     <t>World</t>
   </si>
   <si>
@@ -2133,13 +2157,139 @@
   </si>
   <si>
     <t>Шрі-Ланка</t>
+  </si>
+  <si>
+    <t>vancouver</t>
+  </si>
+  <si>
+    <t>can-british-columbia</t>
+  </si>
+  <si>
+    <t>Ванкувер</t>
+  </si>
+  <si>
+    <t>Vancouver</t>
+  </si>
+  <si>
+    <t>toronto</t>
+  </si>
+  <si>
+    <t>ontario</t>
+  </si>
+  <si>
+    <t>Торонто</t>
+  </si>
+  <si>
+    <t>Toronto</t>
+  </si>
+  <si>
+    <t>ottawa</t>
+  </si>
+  <si>
+    <t>Оттава</t>
+  </si>
+  <si>
+    <t>Ottawa</t>
+  </si>
+  <si>
+    <t>canada</t>
+  </si>
+  <si>
+    <t>британская Колумбия</t>
+  </si>
+  <si>
+    <t>British Columbia</t>
+  </si>
+  <si>
+    <t>Британська Колумбія</t>
+  </si>
+  <si>
+    <t>alberta</t>
+  </si>
+  <si>
+    <t>Альберта</t>
+  </si>
+  <si>
+    <t>Alberta</t>
+  </si>
+  <si>
+    <t>saskatchewan</t>
+  </si>
+  <si>
+    <t>Саскачеван</t>
+  </si>
+  <si>
+    <t>Saskatchewan</t>
+  </si>
+  <si>
+    <t>edmonton</t>
+  </si>
+  <si>
+    <t>Эдмонтон</t>
+  </si>
+  <si>
+    <t>Edmonton</t>
+  </si>
+  <si>
+    <t>Едмонтон</t>
+  </si>
+  <si>
+    <t>manitoba</t>
+  </si>
+  <si>
+    <t>Манитоба</t>
+  </si>
+  <si>
+    <t>Manitoba</t>
+  </si>
+  <si>
+    <t>Манітоба</t>
+  </si>
+  <si>
+    <t>winnipeg</t>
+  </si>
+  <si>
+    <t>Виннипег</t>
+  </si>
+  <si>
+    <t>Winnipeg</t>
+  </si>
+  <si>
+    <t>Вінніпег</t>
+  </si>
+  <si>
+    <t>Онтарио</t>
+  </si>
+  <si>
+    <t>Ontario</t>
+  </si>
+  <si>
+    <t>Онтаріо</t>
+  </si>
+  <si>
+    <t>quebec</t>
+  </si>
+  <si>
+    <t>Квебек</t>
+  </si>
+  <si>
+    <t>Quebec</t>
+  </si>
+  <si>
+    <t>montreal</t>
+  </si>
+  <si>
+    <t>Монреаль</t>
+  </si>
+  <si>
+    <t>Montreal</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="7">
+  <fonts count="5">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -2158,10 +2308,6 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
-    <font>
-      <name val="Arial"/>
-    </font>
-    <font/>
     <font>
       <u/>
       <color rgb="FF000000"/>
@@ -2188,7 +2334,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -2214,12 +2360,6 @@
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -4125,6 +4265,40 @@
         <v>310</v>
       </c>
     </row>
+    <row r="103">
+      <c r="A103" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="D103" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="E103" s="1" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="D104" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="E104" s="1" t="s">
+        <v>318</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -4139,6 +4313,11 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="24.43"/>
+    <col customWidth="1" min="3" max="3" width="29.71"/>
+    <col customWidth="1" min="4" max="4" width="25.29"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
@@ -4159,1950 +4338,2154 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>311</v>
+        <v>319</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>312</v>
+        <v>320</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>311</v>
+        <v>319</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>313</v>
+        <v>321</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>314</v>
+        <v>322</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>315</v>
+        <v>323</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>314</v>
+        <v>322</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>316</v>
+        <v>324</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>317</v>
+        <v>325</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>314</v>
+        <v>322</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>318</v>
+        <v>326</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>317</v>
+        <v>325</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>318</v>
+        <v>326</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>319</v>
+        <v>327</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>314</v>
+        <v>322</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>320</v>
+        <v>328</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>319</v>
+        <v>327</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>321</v>
+        <v>329</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>322</v>
+        <v>330</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>323</v>
+        <v>331</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>322</v>
+        <v>330</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>324</v>
+        <v>332</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>325</v>
+        <v>333</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>326</v>
+        <v>334</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>327</v>
+        <v>335</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>328</v>
+        <v>336</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>329</v>
+        <v>337</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>330</v>
+        <v>338</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>331</v>
+        <v>339</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>330</v>
+        <v>338</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>331</v>
+        <v>339</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>332</v>
+        <v>340</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>330</v>
+        <v>338</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>333</v>
+        <v>341</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>332</v>
+        <v>340</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>333</v>
+        <v>341</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>334</v>
+        <v>342</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>330</v>
+        <v>338</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>335</v>
+        <v>343</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>334</v>
+        <v>342</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>336</v>
+        <v>344</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>337</v>
+        <v>345</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>338</v>
+        <v>346</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>337</v>
+        <v>345</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>338</v>
+        <v>346</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>339</v>
+        <v>347</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>340</v>
+        <v>348</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>339</v>
+        <v>347</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>341</v>
+        <v>349</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>342</v>
+        <v>350</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>343</v>
+        <v>351</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>342</v>
+        <v>350</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>344</v>
+        <v>352</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>345</v>
+        <v>353</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>322</v>
+        <v>330</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>346</v>
+        <v>354</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>345</v>
+        <v>353</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>347</v>
+        <v>355</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>348</v>
+        <v>356</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>349</v>
+        <v>357</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>348</v>
+        <v>356</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>350</v>
+        <v>358</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>351</v>
+        <v>359</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>325</v>
+        <v>333</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>352</v>
+        <v>360</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>351</v>
+        <v>359</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>353</v>
+        <v>361</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>354</v>
+        <v>362</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>322</v>
+        <v>330</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>355</v>
+        <v>363</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>354</v>
+        <v>362</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>356</v>
+        <v>364</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>357</v>
+        <v>365</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>322</v>
+        <v>330</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>358</v>
+        <v>366</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>357</v>
+        <v>365</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>359</v>
+        <v>367</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>360</v>
+        <v>368</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>322</v>
+        <v>330</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>361</v>
+        <v>369</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>360</v>
+        <v>368</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>362</v>
+        <v>370</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>363</v>
+        <v>371</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>322</v>
+        <v>330</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>364</v>
+        <v>372</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>363</v>
+        <v>371</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>365</v>
+        <v>373</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>366</v>
+        <v>374</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>322</v>
+        <v>330</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>367</v>
+        <v>375</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>366</v>
-      </c>
-      <c r="E21" s="8" t="s">
-        <v>368</v>
+        <v>374</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>376</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>369</v>
+        <v>377</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>322</v>
+        <v>330</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>370</v>
+        <v>378</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>369</v>
+        <v>377</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>371</v>
+        <v>379</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>372</v>
+        <v>380</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>322</v>
+        <v>330</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>373</v>
+        <v>381</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>372</v>
+        <v>380</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>374</v>
+        <v>382</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>375</v>
+        <v>383</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>322</v>
+        <v>330</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>376</v>
+        <v>384</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>375</v>
+        <v>383</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>377</v>
+        <v>385</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>378</v>
+        <v>386</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>322</v>
+        <v>330</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>379</v>
+        <v>387</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>378</v>
+        <v>386</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>380</v>
+        <v>388</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>381</v>
+        <v>389</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>322</v>
+        <v>330</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>382</v>
+        <v>390</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>381</v>
+        <v>389</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>383</v>
+        <v>391</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>384</v>
+        <v>392</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>322</v>
+        <v>330</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>385</v>
+        <v>393</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>384</v>
+        <v>392</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>386</v>
+        <v>394</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>387</v>
+        <v>395</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>330</v>
+        <v>338</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>388</v>
+        <v>396</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>387</v>
+        <v>395</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>388</v>
+        <v>396</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>389</v>
+        <v>397</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>390</v>
+        <v>398</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>391</v>
+        <v>399</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>389</v>
+        <v>397</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>392</v>
+        <v>400</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>393</v>
+        <v>401</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>345</v>
+        <v>353</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>394</v>
+        <v>402</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>395</v>
+        <v>403</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>396</v>
+        <v>404</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>397</v>
+        <v>405</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>345</v>
+        <v>353</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>398</v>
+        <v>406</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>399</v>
+        <v>407</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>400</v>
+        <v>408</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>401</v>
+        <v>409</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>345</v>
+        <v>353</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>402</v>
+        <v>410</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>403</v>
+        <v>411</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>402</v>
+        <v>410</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>404</v>
+        <v>412</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>345</v>
+        <v>353</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>405</v>
+        <v>413</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>406</v>
+        <v>414</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>407</v>
+        <v>415</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
-        <v>408</v>
+        <v>416</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>345</v>
+        <v>353</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>409</v>
+        <v>417</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>410</v>
+        <v>418</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>411</v>
+        <v>419</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
-        <v>412</v>
+        <v>420</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>345</v>
+        <v>353</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>413</v>
+        <v>421</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>414</v>
+        <v>422</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>415</v>
+        <v>423</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
-        <v>416</v>
+        <v>424</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>389</v>
+        <v>397</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>417</v>
+        <v>425</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>418</v>
+        <v>426</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>417</v>
+        <v>425</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="s">
-        <v>419</v>
+        <v>427</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>389</v>
+        <v>397</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>420</v>
+        <v>428</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>421</v>
+        <v>429</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>420</v>
+        <v>428</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="s">
-        <v>422</v>
+        <v>430</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>389</v>
+        <v>397</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>423</v>
+        <v>431</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>424</v>
+        <v>432</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>423</v>
+        <v>431</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="s">
-        <v>425</v>
+        <v>433</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>389</v>
+        <v>397</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>426</v>
+        <v>434</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>427</v>
+        <v>435</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>426</v>
+        <v>434</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="s">
-        <v>428</v>
+        <v>436</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>389</v>
+        <v>397</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>429</v>
+        <v>437</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>430</v>
+        <v>438</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>429</v>
+        <v>437</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="s">
-        <v>431</v>
+        <v>439</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>389</v>
+        <v>397</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>432</v>
+        <v>440</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>433</v>
+        <v>441</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>432</v>
+        <v>440</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="s">
-        <v>434</v>
+        <v>442</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>334</v>
+        <v>342</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>435</v>
+        <v>443</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>436</v>
+        <v>444</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>435</v>
+        <v>443</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="s">
-        <v>437</v>
+        <v>445</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>438</v>
+        <v>446</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>439</v>
+        <v>447</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>440</v>
+        <v>448</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>439</v>
+        <v>447</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="s">
-        <v>441</v>
+        <v>449</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>438</v>
+        <v>446</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>442</v>
+        <v>450</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>443</v>
+        <v>451</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>442</v>
+        <v>450</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="s">
-        <v>444</v>
+        <v>452</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>438</v>
+        <v>446</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>445</v>
+        <v>453</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>446</v>
+        <v>454</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>447</v>
+        <v>455</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="s">
-        <v>448</v>
+        <v>456</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>438</v>
+        <v>446</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>449</v>
+        <v>457</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>450</v>
+        <v>458</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>449</v>
+        <v>457</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="s">
-        <v>451</v>
+        <v>459</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>452</v>
+        <v>460</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>453</v>
+        <v>461</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>454</v>
+        <v>462</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>455</v>
+        <v>463</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="s">
-        <v>456</v>
+        <v>464</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>390</v>
+        <v>398</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>457</v>
+        <v>465</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>458</v>
+        <v>466</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>459</v>
+        <v>467</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="s">
-        <v>460</v>
+        <v>468</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>390</v>
+        <v>398</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>461</v>
+        <v>469</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>462</v>
+        <v>470</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>463</v>
+        <v>471</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="s">
-        <v>464</v>
+        <v>472</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>390</v>
+        <v>398</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>465</v>
+        <v>473</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>466</v>
+        <v>474</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>465</v>
+        <v>473</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="s">
-        <v>467</v>
+        <v>475</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>390</v>
+        <v>398</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>468</v>
+        <v>476</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>469</v>
+        <v>477</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>470</v>
+        <v>478</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="s">
-        <v>390</v>
+        <v>398</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>314</v>
+        <v>322</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>471</v>
+        <v>479</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>472</v>
+        <v>480</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>473</v>
+        <v>481</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="s">
-        <v>474</v>
+        <v>482</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>322</v>
+        <v>330</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>475</v>
+        <v>483</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>476</v>
+        <v>484</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>477</v>
+        <v>485</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="s">
-        <v>478</v>
+        <v>486</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>342</v>
+        <v>350</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>479</v>
+        <v>487</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>480</v>
+        <v>488</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>481</v>
+        <v>489</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="s">
-        <v>482</v>
+        <v>490</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>342</v>
-      </c>
-      <c r="C55" s="9" t="s">
-        <v>483</v>
-      </c>
-      <c r="D55" s="9" t="s">
-        <v>484</v>
+        <v>350</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>492</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>485</v>
+        <v>493</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="s">
-        <v>486</v>
+        <v>494</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>342</v>
-      </c>
-      <c r="C56" s="9" t="s">
-        <v>487</v>
-      </c>
-      <c r="D56" s="9" t="s">
-        <v>488</v>
+        <v>350</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>495</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>496</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>489</v>
+        <v>497</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="s">
-        <v>490</v>
+        <v>498</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>326</v>
+        <v>334</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>491</v>
+        <v>499</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>492</v>
+        <v>500</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>493</v>
+        <v>501</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="s">
-        <v>494</v>
+        <v>502</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>326</v>
+        <v>334</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>495</v>
+        <v>503</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>496</v>
+        <v>504</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>497</v>
+        <v>505</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="s">
-        <v>498</v>
+        <v>506</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>326</v>
+        <v>334</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>499</v>
+        <v>507</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>500</v>
+        <v>508</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>501</v>
+        <v>509</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="s">
-        <v>502</v>
+        <v>510</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>326</v>
+        <v>334</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>503</v>
+        <v>511</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>504</v>
-      </c>
-      <c r="E60" s="9" t="s">
-        <v>505</v>
+        <v>512</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>513</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="s">
-        <v>506</v>
+        <v>514</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>326</v>
+        <v>334</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>507</v>
+        <v>515</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>508</v>
+        <v>516</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>509</v>
+        <v>517</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="s">
-        <v>510</v>
+        <v>518</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>511</v>
+        <v>519</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>512</v>
+        <v>520</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>513</v>
+        <v>521</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>514</v>
+        <v>522</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="s">
-        <v>515</v>
+        <v>523</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>326</v>
+        <v>334</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>516</v>
+        <v>524</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>517</v>
+        <v>525</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>518</v>
+        <v>526</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="s">
-        <v>519</v>
+        <v>527</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>326</v>
+        <v>334</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>520</v>
+        <v>528</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>521</v>
+        <v>529</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>522</v>
+        <v>530</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="s">
-        <v>523</v>
+        <v>531</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>326</v>
+        <v>334</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>524</v>
+        <v>532</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>525</v>
+        <v>533</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>526</v>
+        <v>534</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="s">
-        <v>527</v>
+        <v>535</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>326</v>
+        <v>334</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>528</v>
+        <v>536</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>529</v>
+        <v>537</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>530</v>
+        <v>538</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="s">
-        <v>531</v>
+        <v>539</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>326</v>
+        <v>334</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>532</v>
+        <v>540</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>533</v>
+        <v>541</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>534</v>
+        <v>542</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="s">
-        <v>535</v>
+        <v>543</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>326</v>
+        <v>334</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>536</v>
+        <v>544</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>537</v>
+        <v>545</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>538</v>
+        <v>546</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="s">
-        <v>539</v>
+        <v>547</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>326</v>
+        <v>334</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>540</v>
+        <v>548</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>541</v>
+        <v>549</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>542</v>
+        <v>550</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="s">
-        <v>543</v>
+        <v>551</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>326</v>
+        <v>334</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>544</v>
+        <v>552</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>545</v>
+        <v>553</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>546</v>
+        <v>554</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="s">
-        <v>547</v>
+        <v>555</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>326</v>
+        <v>334</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>548</v>
+        <v>556</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>549</v>
+        <v>557</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>550</v>
+        <v>558</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="s">
-        <v>551</v>
+        <v>559</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>326</v>
+        <v>334</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>552</v>
+        <v>560</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>553</v>
+        <v>561</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>554</v>
+        <v>562</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="s">
-        <v>555</v>
+        <v>563</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>556</v>
+        <v>564</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>557</v>
+        <v>565</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>558</v>
+        <v>566</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>559</v>
+        <v>567</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="s">
-        <v>560</v>
+        <v>568</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>326</v>
+        <v>334</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>561</v>
+        <v>569</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>562</v>
+        <v>570</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>563</v>
+        <v>571</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="s">
+        <v>572</v>
+      </c>
+      <c r="B75" s="1" t="s">
         <v>564</v>
       </c>
-      <c r="B75" s="1" t="s">
-        <v>556</v>
-      </c>
       <c r="C75" s="1" t="s">
-        <v>565</v>
-      </c>
-      <c r="D75" s="9" t="s">
-        <v>566</v>
+        <v>573</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>574</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>566</v>
+        <v>574</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="s">
-        <v>567</v>
+        <v>575</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>314</v>
+        <v>322</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>568</v>
-      </c>
-      <c r="D76" s="9" t="s">
-        <v>569</v>
+        <v>576</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>577</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>570</v>
+        <v>578</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="s">
-        <v>571</v>
+        <v>579</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>556</v>
+        <v>564</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>572</v>
-      </c>
-      <c r="D77" s="9" t="s">
-        <v>572</v>
+        <v>580</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>580</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>572</v>
+        <v>580</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="s">
-        <v>573</v>
+        <v>581</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>556</v>
+        <v>564</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>574</v>
-      </c>
-      <c r="D78" s="9" t="s">
-        <v>575</v>
+        <v>582</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>583</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>575</v>
+        <v>583</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="s">
-        <v>576</v>
+        <v>584</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>556</v>
+        <v>564</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>577</v>
-      </c>
-      <c r="D79" s="9" t="s">
-        <v>578</v>
+        <v>585</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>586</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>578</v>
+        <v>586</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="s">
-        <v>579</v>
+        <v>587</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>556</v>
+        <v>564</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>580</v>
-      </c>
-      <c r="D80" s="9" t="s">
-        <v>581</v>
+        <v>588</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>589</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>581</v>
+        <v>589</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="s">
-        <v>582</v>
+        <v>590</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>556</v>
+        <v>564</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>583</v>
-      </c>
-      <c r="D81" s="9" t="s">
-        <v>584</v>
+        <v>591</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>592</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>584</v>
+        <v>592</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="s">
-        <v>585</v>
+        <v>593</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>325</v>
+        <v>333</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>586</v>
-      </c>
-      <c r="D82" s="9" t="s">
-        <v>587</v>
+        <v>594</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>595</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>588</v>
+        <v>596</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="s">
-        <v>589</v>
+        <v>597</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>511</v>
+        <v>519</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>590</v>
-      </c>
-      <c r="D83" s="9" t="s">
-        <v>590</v>
+        <v>598</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>598</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>590</v>
+        <v>598</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="s">
-        <v>591</v>
+        <v>599</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>556</v>
+        <v>564</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>592</v>
-      </c>
-      <c r="D84" s="9" t="s">
-        <v>593</v>
+        <v>600</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>601</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>593</v>
+        <v>601</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="s">
-        <v>594</v>
+        <v>602</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>556</v>
+        <v>564</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>595</v>
-      </c>
-      <c r="D85" s="9" t="s">
-        <v>596</v>
+        <v>603</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>604</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>596</v>
+        <v>604</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="s">
-        <v>597</v>
+        <v>605</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>556</v>
+        <v>564</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>598</v>
-      </c>
-      <c r="D86" s="9" t="s">
-        <v>599</v>
+        <v>606</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>607</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>599</v>
+        <v>607</v>
       </c>
     </row>
     <row r="87">
-      <c r="A87" s="10" t="s">
-        <v>600</v>
+      <c r="A87" s="8" t="s">
+        <v>608</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>556</v>
+        <v>564</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>601</v>
-      </c>
-      <c r="D87" s="9" t="s">
-        <v>602</v>
+        <v>609</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>610</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>602</v>
+        <v>610</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="6" t="s">
-        <v>603</v>
+        <v>611</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>556</v>
+        <v>564</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>604</v>
-      </c>
-      <c r="D88" s="9" t="s">
-        <v>605</v>
+        <v>612</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>613</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>605</v>
+        <v>613</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="6" t="s">
-        <v>606</v>
+        <v>614</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>556</v>
+        <v>564</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>607</v>
-      </c>
-      <c r="D89" s="9" t="s">
-        <v>608</v>
+        <v>615</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>616</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>608</v>
+        <v>616</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="s">
-        <v>609</v>
+        <v>617</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>556</v>
+        <v>564</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>610</v>
-      </c>
-      <c r="D90" s="9" t="s">
-        <v>611</v>
+        <v>618</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>619</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>611</v>
+        <v>619</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="1" t="s">
-        <v>612</v>
+        <v>620</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>390</v>
+        <v>398</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>613</v>
-      </c>
-      <c r="D91" s="9" t="s">
-        <v>614</v>
+        <v>621</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>622</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>615</v>
+        <v>623</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="1" t="s">
-        <v>616</v>
+        <v>624</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>390</v>
+        <v>398</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>617</v>
-      </c>
-      <c r="D92" s="9" t="s">
-        <v>618</v>
+        <v>625</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>626</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>619</v>
+        <v>627</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="1" t="s">
-        <v>620</v>
+        <v>628</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>326</v>
+        <v>334</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>621</v>
-      </c>
-      <c r="D93" s="9" t="s">
-        <v>622</v>
+        <v>629</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>630</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>623</v>
+        <v>631</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="1" t="s">
-        <v>624</v>
+        <v>632</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>556</v>
+        <v>564</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>625</v>
-      </c>
-      <c r="D94" s="9" t="s">
-        <v>626</v>
+        <v>633</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>634</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>626</v>
+        <v>634</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="1" t="s">
-        <v>627</v>
+        <v>635</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>511</v>
+        <v>519</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>628</v>
-      </c>
-      <c r="D95" s="9" t="s">
-        <v>629</v>
+        <v>636</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>637</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>630</v>
+        <v>638</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="1" t="s">
-        <v>631</v>
+        <v>639</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>390</v>
+        <v>398</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>632</v>
-      </c>
-      <c r="D96" s="9" t="s">
-        <v>633</v>
+        <v>640</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>641</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>634</v>
+        <v>642</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="1" t="s">
-        <v>635</v>
+        <v>643</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>390</v>
+        <v>398</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>636</v>
-      </c>
-      <c r="D97" s="9" t="s">
-        <v>637</v>
+        <v>644</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>645</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>638</v>
+        <v>646</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="1" t="s">
-        <v>639</v>
+        <v>647</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>556</v>
+        <v>564</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>640</v>
-      </c>
-      <c r="D98" s="9" t="s">
-        <v>640</v>
+        <v>648</v>
+      </c>
+      <c r="D98" s="1" t="s">
+        <v>648</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>640</v>
+        <v>648</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="1" t="s">
-        <v>641</v>
+        <v>649</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>326</v>
+        <v>334</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>642</v>
-      </c>
-      <c r="D99" s="9" t="s">
-        <v>643</v>
+        <v>650</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>651</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>644</v>
+        <v>652</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="1" t="s">
-        <v>645</v>
+        <v>653</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>342</v>
+        <v>350</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>646</v>
-      </c>
-      <c r="D100" s="9" t="s">
-        <v>647</v>
+        <v>654</v>
+      </c>
+      <c r="D100" s="1" t="s">
+        <v>655</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>648</v>
+        <v>656</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="1" t="s">
-        <v>649</v>
+        <v>657</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>326</v>
+        <v>334</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>650</v>
-      </c>
-      <c r="D101" s="9" t="s">
-        <v>651</v>
+        <v>658</v>
+      </c>
+      <c r="D101" s="1" t="s">
+        <v>659</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>652</v>
+        <v>660</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="1" t="s">
-        <v>653</v>
+        <v>661</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>556</v>
+        <v>564</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>654</v>
-      </c>
-      <c r="D102" s="9" t="s">
-        <v>655</v>
+        <v>662</v>
+      </c>
+      <c r="D102" s="1" t="s">
+        <v>663</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>656</v>
+        <v>664</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="1" t="s">
-        <v>657</v>
+        <v>665</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>326</v>
+        <v>334</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>658</v>
-      </c>
-      <c r="D103" s="9" t="s">
-        <v>659</v>
+        <v>666</v>
+      </c>
+      <c r="D103" s="1" t="s">
+        <v>667</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>660</v>
+        <v>668</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="6" t="s">
-        <v>661</v>
+        <v>669</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>326</v>
+        <v>334</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>662</v>
-      </c>
-      <c r="D104" s="9" t="s">
-        <v>663</v>
+        <v>670</v>
+      </c>
+      <c r="D104" s="1" t="s">
+        <v>671</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>664</v>
+        <v>672</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="1" t="s">
-        <v>665</v>
+        <v>673</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>556</v>
+        <v>564</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>666</v>
-      </c>
-      <c r="D105" s="9" t="s">
-        <v>667</v>
+        <v>674</v>
+      </c>
+      <c r="D105" s="1" t="s">
+        <v>675</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>667</v>
+        <v>675</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="6" t="s">
-        <v>668</v>
+        <v>676</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>556</v>
+        <v>564</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>669</v>
-      </c>
-      <c r="D106" s="9" t="s">
-        <v>670</v>
+        <v>677</v>
+      </c>
+      <c r="D106" s="1" t="s">
+        <v>678</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>670</v>
+        <v>678</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="6" t="s">
-        <v>671</v>
+        <v>679</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>511</v>
+        <v>519</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>672</v>
-      </c>
-      <c r="D107" s="9" t="s">
-        <v>673</v>
+        <v>680</v>
+      </c>
+      <c r="D107" s="1" t="s">
+        <v>681</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>674</v>
+        <v>682</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="1" t="s">
-        <v>675</v>
+        <v>683</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>511</v>
+        <v>519</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>676</v>
-      </c>
-      <c r="D108" s="9" t="s">
-        <v>677</v>
+        <v>684</v>
+      </c>
+      <c r="D108" s="1" t="s">
+        <v>685</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>678</v>
+        <v>686</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="1" t="s">
-        <v>679</v>
+        <v>687</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>556</v>
+        <v>564</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>680</v>
-      </c>
-      <c r="D109" s="9" t="s">
-        <v>680</v>
+        <v>688</v>
+      </c>
+      <c r="D109" s="1" t="s">
+        <v>688</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>680</v>
+        <v>688</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="6" t="s">
-        <v>681</v>
+        <v>689</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>556</v>
+        <v>564</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>682</v>
-      </c>
-      <c r="D110" s="9" t="s">
-        <v>682</v>
+        <v>690</v>
+      </c>
+      <c r="D110" s="1" t="s">
+        <v>690</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>682</v>
+        <v>690</v>
       </c>
     </row>
     <row r="111">
-      <c r="A111" s="11" t="s">
-        <v>683</v>
+      <c r="A111" s="9" t="s">
+        <v>691</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>556</v>
+        <v>564</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>684</v>
-      </c>
-      <c r="D111" s="9" t="s">
-        <v>685</v>
+        <v>692</v>
+      </c>
+      <c r="D111" s="1" t="s">
+        <v>693</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>685</v>
+        <v>693</v>
       </c>
     </row>
     <row r="112">
-      <c r="A112" s="11" t="s">
-        <v>686</v>
+      <c r="A112" s="9" t="s">
+        <v>694</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>556</v>
+        <v>564</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>687</v>
-      </c>
-      <c r="D112" s="9" t="s">
-        <v>688</v>
+        <v>695</v>
+      </c>
+      <c r="D112" s="1" t="s">
+        <v>696</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>688</v>
+        <v>696</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="6" t="s">
-        <v>689</v>
+        <v>697</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>556</v>
+        <v>564</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>690</v>
-      </c>
-      <c r="D113" s="9" t="s">
-        <v>691</v>
+        <v>698</v>
+      </c>
+      <c r="D113" s="1" t="s">
+        <v>699</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>691</v>
+        <v>699</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="6" t="s">
-        <v>692</v>
+        <v>700</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>556</v>
+        <v>564</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>693</v>
-      </c>
-      <c r="D114" s="9" t="s">
-        <v>694</v>
+        <v>701</v>
+      </c>
+      <c r="D114" s="1" t="s">
+        <v>702</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>694</v>
+        <v>702</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="6" t="s">
-        <v>695</v>
+        <v>703</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>556</v>
+        <v>564</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>696</v>
-      </c>
-      <c r="D115" s="9" t="s">
-        <v>697</v>
+        <v>704</v>
+      </c>
+      <c r="D115" s="1" t="s">
+        <v>705</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>698</v>
+        <v>706</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="1" t="s">
-        <v>699</v>
+        <v>707</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>326</v>
+        <v>334</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>700</v>
-      </c>
-      <c r="D116" s="9" t="s">
-        <v>701</v>
+        <v>708</v>
+      </c>
+      <c r="D116" s="1" t="s">
+        <v>709</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>702</v>
+        <v>710</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="1" t="s">
-        <v>703</v>
+        <v>711</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>390</v>
+        <v>398</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>704</v>
-      </c>
-      <c r="D117" s="9" t="s">
-        <v>705</v>
+        <v>712</v>
+      </c>
+      <c r="D117" s="1" t="s">
+        <v>713</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>706</v>
+        <v>714</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="1" t="s">
+        <v>715</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>716</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>717</v>
+      </c>
+      <c r="D118" s="1" t="s">
+        <v>718</v>
+      </c>
+      <c r="E118" s="1" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" s="1" t="s">
+        <v>719</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>720</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>721</v>
+      </c>
+      <c r="D119" s="1" t="s">
+        <v>722</v>
+      </c>
+      <c r="E119" s="1" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" s="1" t="s">
+        <v>723</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>720</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>724</v>
+      </c>
+      <c r="D120" s="1" t="s">
+        <v>725</v>
+      </c>
+      <c r="E120" s="1" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" s="1" t="s">
+        <v>716</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>726</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>727</v>
+      </c>
+      <c r="D121" s="1" t="s">
+        <v>728</v>
+      </c>
+      <c r="E121" s="1" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>726</v>
+      </c>
+      <c r="C122" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D122" s="1" t="s">
+        <v>732</v>
+      </c>
+      <c r="E122" s="1" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" s="1" t="s">
+        <v>733</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>726</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>734</v>
+      </c>
+      <c r="D123" s="1" t="s">
+        <v>735</v>
+      </c>
+      <c r="E123" s="1" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" s="1" t="s">
+        <v>736</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>737</v>
+      </c>
+      <c r="D124" s="1" t="s">
+        <v>738</v>
+      </c>
+      <c r="E124" s="1" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" s="1" t="s">
+        <v>740</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>726</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>741</v>
+      </c>
+      <c r="D125" s="1" t="s">
+        <v>742</v>
+      </c>
+      <c r="E125" s="1" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" s="1" t="s">
+        <v>744</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>740</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>745</v>
+      </c>
+      <c r="D126" s="1" t="s">
+        <v>746</v>
+      </c>
+      <c r="E126" s="1" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" s="1" t="s">
+        <v>720</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>726</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>748</v>
+      </c>
+      <c r="D127" s="1" t="s">
+        <v>749</v>
+      </c>
+      <c r="E127" s="1" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" s="1" t="s">
+        <v>751</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>726</v>
+      </c>
+      <c r="C128" s="1" t="s">
+        <v>752</v>
+      </c>
+      <c r="D128" s="1" t="s">
+        <v>753</v>
+      </c>
+      <c r="E128" s="1" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" s="1" t="s">
+        <v>754</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>751</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>755</v>
+      </c>
+      <c r="D129" s="1" t="s">
+        <v>756</v>
+      </c>
+      <c r="E129" s="1" t="s">
+        <v>755</v>
       </c>
     </row>
   </sheetData>

</xml_diff>